<commit_message>
Update WGL bus bay data
</commit_message>
<xml_diff>
--- a/excel/bus/bays/Bus Bays.xlsx
+++ b/excel/bus/bays/Bus Bays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardyeung/Projects/TVData/excel/bus/bays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3CDF80-F1B8-204E-8D61-C240FE3A6B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459655A0-1D1D-5540-9348-7E51E9FCFA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{1F3FC56B-3071-1747-8E11-6356A10C0FCD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="109">
   <si>
     <t>E</t>
   </si>
@@ -351,6 +351,18 @@
   </si>
   <si>
     <t>Swanston st stop</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Warragul Station/Alfred St (Warragul)</t>
   </si>
 </sst>
 </file>
@@ -1221,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
-  <dimension ref="A1:D416"/>
+  <dimension ref="A1:D419"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1232,6 +1244,7 @@
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -5838,6 +5851,39 @@
       </c>
       <c r="C416" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <v>47668</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C417" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A418">
+        <v>47669</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C418" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A419">
+        <v>47670</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C419" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -5851,5 +5897,8 @@
     <sortCondition ref="B2:B416"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="B417:B419" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update BMH & La Trobe Uni bus bays
</commit_message>
<xml_diff>
--- a/excel/bus/bays/Bus Bays.xlsx
+++ b/excel/bus/bays/Bus Bays.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardyeung/Projects/TVData/excel/bus/bays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459655A0-1D1D-5540-9348-7E51E9FCFA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6C1AB7-9FFC-F047-AA03-387A96B8A9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{1F3FC56B-3071-1747-8E11-6356A10C0FCD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F3FC56B-3071-1747-8E11-6356A10C0FCD}"/>
   </bookViews>
   <sheets>
     <sheet name="bays" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bays!$A$1:$C$416</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bays!$A$1:$C$415</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="117">
   <si>
     <t>E</t>
   </si>
@@ -363,6 +363,30 @@
   </si>
   <si>
     <t>Warragul Station/Alfred St (Warragul)</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>La Trobe Uni Thomas Cherry Building/Science Dr (Bundoora)</t>
+  </si>
+  <si>
+    <t>La Trobe University (Bundoora)</t>
+  </si>
+  <si>
+    <t>Bus interchange</t>
+  </si>
+  <si>
+    <t>301 stop</t>
+  </si>
+  <si>
+    <t>Bay 3 is Up TRBS, unsigned</t>
+  </si>
+  <si>
+    <t>coach and TRBS stop</t>
   </si>
 </sst>
 </file>
@@ -852,12 +876,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1233,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
-  <dimension ref="A1:D419"/>
+  <dimension ref="A1:D426"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A269" workbookViewId="0">
+      <selection activeCell="C280" sqref="C280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1244,7 +1269,7 @@
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1263,12 +1288,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>48832</v>
+        <v>37707</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1279,7 +1304,7 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1290,7 +1315,7 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1301,8 +1326,11 @@
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2661,7 +2689,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>19483</v>
       </c>
@@ -2672,7 +2700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>19273</v>
       </c>
@@ -2683,7 +2711,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>19485</v>
       </c>
@@ -2694,7 +2722,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>19476</v>
       </c>
@@ -2705,7 +2733,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>19486</v>
       </c>
@@ -2716,7 +2744,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>19488</v>
       </c>
@@ -2727,7 +2755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>48851</v>
       </c>
@@ -2738,7 +2766,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>48850</v>
       </c>
@@ -2749,7 +2777,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>43683</v>
       </c>
@@ -2760,7 +2788,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>42635</v>
       </c>
@@ -2770,8 +2798,11 @@
       <c r="C138" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>21490</v>
       </c>
@@ -2782,7 +2813,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>20799</v>
       </c>
@@ -2793,7 +2824,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>21492</v>
       </c>
@@ -2804,7 +2835,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>48397</v>
       </c>
@@ -2815,7 +2846,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>48396</v>
       </c>
@@ -2826,7 +2857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>46332</v>
       </c>
@@ -3541,7 +3572,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>51589</v>
       </c>
@@ -3552,7 +3583,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>51590</v>
       </c>
@@ -3563,7 +3594,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>40359</v>
       </c>
@@ -3574,7 +3605,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>19637</v>
       </c>
@@ -3585,7 +3616,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>19636</v>
       </c>
@@ -3596,7 +3627,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>19635</v>
       </c>
@@ -3607,7 +3638,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>19634</v>
       </c>
@@ -3618,7 +3649,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>40358</v>
       </c>
@@ -3629,7 +3660,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>19632</v>
       </c>
@@ -3640,7 +3671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>19631</v>
       </c>
@@ -3651,7 +3682,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>19630</v>
       </c>
@@ -3662,7 +3693,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>19629</v>
       </c>
@@ -3673,576 +3704,582 @@
         <v>31</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221">
-        <v>20947</v>
-      </c>
-      <c r="B221" s="1">
-        <v>4</v>
+        <v>48036</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C221" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="D221" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222">
-        <v>20951</v>
-      </c>
-      <c r="B222" s="1">
-        <v>5</v>
-      </c>
-      <c r="C222" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C222" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223">
-        <v>20942</v>
-      </c>
-      <c r="B223" s="1">
-        <v>1</v>
+        <v>768</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C223" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224">
-        <v>20945</v>
-      </c>
-      <c r="B224" s="1">
-        <v>2</v>
+        <v>6664</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C224" t="s">
-        <v>37</v>
+        <v>112</v>
+      </c>
+      <c r="D224" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225">
-        <v>20944</v>
-      </c>
-      <c r="B225" s="1">
-        <v>3</v>
+        <v>6665</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C225" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226">
-        <v>23444</v>
-      </c>
-      <c r="B226" s="1">
-        <v>11</v>
+        <v>6666</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C226" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227">
-        <v>22609</v>
-      </c>
-      <c r="B227" s="1">
-        <v>12</v>
+        <v>6667</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C227" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228">
-        <v>40954</v>
-      </c>
-      <c r="B228" s="1">
-        <v>6</v>
+        <v>6668</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C228" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229">
-        <v>40400</v>
+        <v>20947</v>
       </c>
       <c r="B229" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C229" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230">
-        <v>21170</v>
+        <v>20951</v>
       </c>
       <c r="B230" s="1">
-        <v>8</v>
-      </c>
-      <c r="C230" t="s">
-        <v>50</v>
+        <v>5</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231">
-        <v>28196</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>13</v>
+        <v>20942</v>
+      </c>
+      <c r="B231" s="1">
+        <v>1</v>
       </c>
       <c r="C231" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232">
-        <v>28197</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>15</v>
+        <v>20945</v>
+      </c>
+      <c r="B232" s="1">
+        <v>2</v>
       </c>
       <c r="C232" t="s">
-        <v>67</v>
-      </c>
-      <c r="D232" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233">
-        <v>28198</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>14</v>
+        <v>20944</v>
+      </c>
+      <c r="B233" s="1">
+        <v>3</v>
       </c>
       <c r="C233" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234">
-        <v>28199</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>12</v>
+        <v>23444</v>
+      </c>
+      <c r="B234" s="1">
+        <v>11</v>
       </c>
       <c r="C234" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235">
-        <v>28191</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>2</v>
+        <v>22609</v>
+      </c>
+      <c r="B235" s="1">
+        <v>12</v>
       </c>
       <c r="C235" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236">
-        <v>28192</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>3</v>
+        <v>40954</v>
+      </c>
+      <c r="B236" s="1">
+        <v>6</v>
       </c>
       <c r="C236" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237">
-        <v>28193</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>4</v>
+        <v>40400</v>
+      </c>
+      <c r="B237" s="1">
+        <v>7</v>
       </c>
       <c r="C237" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238">
-        <v>28194</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>1</v>
+        <v>21170</v>
+      </c>
+      <c r="B238" s="1">
+        <v>8</v>
       </c>
       <c r="C238" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239">
-        <v>28195</v>
+        <v>28196</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C239" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240">
-        <v>52172</v>
-      </c>
-      <c r="B240" s="1">
-        <v>4</v>
-      </c>
-      <c r="C240" s="2" t="s">
-        <v>84</v>
+        <v>28197</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C240" t="s">
+        <v>67</v>
+      </c>
+      <c r="D240" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241">
-        <v>47996</v>
-      </c>
-      <c r="B241" s="1">
-        <v>16</v>
+        <v>28198</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C241" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242">
-        <v>47997</v>
-      </c>
-      <c r="B242" s="1">
-        <v>17</v>
+        <v>28199</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C242" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243">
-        <v>47998</v>
-      </c>
-      <c r="B243" s="1">
-        <v>18</v>
+        <v>28191</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C243" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244">
-        <v>47999</v>
-      </c>
-      <c r="B244" s="1">
-        <v>19</v>
+        <v>28192</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C244" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245">
-        <v>21183</v>
-      </c>
-      <c r="B245" s="1">
-        <v>1</v>
+        <v>28193</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C245" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246">
-        <v>21184</v>
-      </c>
-      <c r="B246" s="1">
-        <v>2</v>
+        <v>28194</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C246" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247">
-        <v>21185</v>
-      </c>
-      <c r="B247" s="1">
-        <v>3</v>
+        <v>28195</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C247" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248">
-        <v>21131</v>
+        <v>52172</v>
       </c>
       <c r="B248" s="1">
         <v>4</v>
       </c>
-      <c r="C248" t="s">
-        <v>48</v>
+      <c r="C248" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249">
-        <v>21132</v>
+        <v>47996</v>
       </c>
       <c r="B249" s="1">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C249" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250">
-        <v>27577</v>
+        <v>47997</v>
       </c>
       <c r="B250" s="1">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C250" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251">
-        <v>51732</v>
+        <v>47998</v>
       </c>
       <c r="B251" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C251" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252">
-        <v>51731</v>
+        <v>47999</v>
       </c>
       <c r="B252" s="1">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C252" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253">
-        <v>51733</v>
+        <v>21183</v>
       </c>
       <c r="B253" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C253" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254">
-        <v>51734</v>
+        <v>21184</v>
       </c>
       <c r="B254" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C254" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255">
-        <v>47111</v>
+        <v>21185</v>
       </c>
       <c r="B255" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C255" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256">
-        <v>47112</v>
+        <v>21131</v>
       </c>
       <c r="B256" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C256" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257">
-        <v>47113</v>
+        <v>21132</v>
       </c>
       <c r="B257" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C257" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258">
-        <v>21048</v>
+        <v>27577</v>
       </c>
       <c r="B258" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C258" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259">
-        <v>47109</v>
+        <v>51732</v>
       </c>
       <c r="B259" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C259" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260">
-        <v>47110</v>
+        <v>51731</v>
       </c>
       <c r="B260" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C260" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261">
-        <v>47168</v>
+        <v>51733</v>
       </c>
       <c r="B261" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C261" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262">
-        <v>35756</v>
-      </c>
-      <c r="B262" s="1" t="s">
-        <v>2</v>
+        <v>51734</v>
+      </c>
+      <c r="B262" s="1">
+        <v>4</v>
       </c>
       <c r="C262" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263">
-        <v>35822</v>
-      </c>
-      <c r="B263" s="1" t="s">
-        <v>3</v>
+        <v>47111</v>
+      </c>
+      <c r="B263" s="1">
+        <v>5</v>
       </c>
       <c r="C263" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264">
-        <v>48368</v>
-      </c>
-      <c r="B264" s="1" t="s">
-        <v>2</v>
+        <v>47112</v>
+      </c>
+      <c r="B264" s="1">
+        <v>6</v>
       </c>
       <c r="C264" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265">
-        <v>22969</v>
-      </c>
-      <c r="B265" s="1" t="s">
-        <v>3</v>
+        <v>47113</v>
+      </c>
+      <c r="B265" s="1">
+        <v>7</v>
       </c>
       <c r="C265" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266">
-        <v>21611</v>
-      </c>
-      <c r="B266" s="1" t="s">
-        <v>4</v>
+        <v>21048</v>
+      </c>
+      <c r="B266" s="1">
+        <v>1</v>
       </c>
       <c r="C266" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267">
-        <v>19815</v>
-      </c>
-      <c r="B267" s="1" t="s">
-        <v>1</v>
+        <v>47109</v>
+      </c>
+      <c r="B267" s="1">
+        <v>2</v>
       </c>
       <c r="C267" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268">
-        <v>19814</v>
-      </c>
-      <c r="B268" s="1" t="s">
-        <v>0</v>
+        <v>47110</v>
+      </c>
+      <c r="B268" s="1">
+        <v>3</v>
       </c>
       <c r="C268" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269">
-        <v>48471</v>
-      </c>
-      <c r="B269" s="1" t="s">
-        <v>13</v>
+        <v>47168</v>
+      </c>
+      <c r="B269" s="1">
+        <v>4</v>
       </c>
       <c r="C269" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270">
-        <v>48473</v>
+        <v>35756</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C270" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271">
-        <v>48474</v>
+        <v>35822</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C271" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272">
-        <v>19813</v>
+        <v>48368</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C272" t="s">
         <v>34</v>
@@ -4250,10 +4287,10 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273">
-        <v>19812</v>
+        <v>22969</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C273" t="s">
         <v>34</v>
@@ -4261,10 +4298,10 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274">
-        <v>19811</v>
+        <v>21611</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C274" t="s">
         <v>34</v>
@@ -4272,10 +4309,10 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275">
-        <v>19810</v>
+        <v>19815</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C275" t="s">
         <v>34</v>
@@ -4283,10 +4320,10 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276">
-        <v>19809</v>
+        <v>19814</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C276" t="s">
         <v>34</v>
@@ -4294,140 +4331,140 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277">
-        <v>19808</v>
+        <v>48471</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C277" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C277" t="s">
         <v>34</v>
-      </c>
-      <c r="D277" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278">
-        <v>19807</v>
+        <v>48473</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C278" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C278" t="s">
         <v>34</v>
-      </c>
-      <c r="D278" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279">
-        <v>19806</v>
+        <v>48474</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C279" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C279" t="s">
         <v>34</v>
-      </c>
-      <c r="D279" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280">
-        <v>18776</v>
-      </c>
-      <c r="B280" s="1">
-        <v>1</v>
+        <v>19813</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C280" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281">
-        <v>18777</v>
-      </c>
-      <c r="B281" s="1">
-        <v>2</v>
+        <v>19812</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C281" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282">
-        <v>18778</v>
-      </c>
-      <c r="B282" s="1">
-        <v>3</v>
+        <v>19811</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C282" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283">
-        <v>18779</v>
-      </c>
-      <c r="B283" s="1">
-        <v>4</v>
+        <v>19810</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C283" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284">
-        <v>18780</v>
-      </c>
-      <c r="B284" s="1">
-        <v>5</v>
+        <v>19809</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C284" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285">
-        <v>18848</v>
-      </c>
-      <c r="B285" s="1">
-        <v>6</v>
-      </c>
-      <c r="C285" t="s">
-        <v>26</v>
+        <v>19808</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D285" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286">
-        <v>18849</v>
-      </c>
-      <c r="B286" s="1">
-        <v>7</v>
-      </c>
-      <c r="C286" t="s">
-        <v>26</v>
+        <v>19807</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D286" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287">
-        <v>18850</v>
-      </c>
-      <c r="B287" s="1">
-        <v>8</v>
-      </c>
-      <c r="C287" t="s">
-        <v>26</v>
+        <v>19806</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D287" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288">
-        <v>47703</v>
+        <v>18776</v>
       </c>
       <c r="B288" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C288" t="s">
         <v>26</v>
@@ -4435,236 +4472,236 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289">
-        <v>21294</v>
-      </c>
-      <c r="B289" s="1" t="s">
+        <v>18777</v>
+      </c>
+      <c r="B289" s="1">
         <v>2</v>
       </c>
       <c r="C289" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290">
-        <v>42981</v>
-      </c>
-      <c r="B290" s="1" t="s">
+        <v>18778</v>
+      </c>
+      <c r="B290" s="1">
         <v>3</v>
       </c>
-      <c r="C290" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D290" t="s">
-        <v>101</v>
+      <c r="C290" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291">
-        <v>42982</v>
-      </c>
-      <c r="B291" s="1" t="s">
+        <v>18779</v>
+      </c>
+      <c r="B291" s="1">
         <v>4</v>
       </c>
-      <c r="C291" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D291" t="s">
-        <v>101</v>
+      <c r="C291" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292">
-        <v>32029</v>
+        <v>18780</v>
       </c>
       <c r="B292" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C292" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293">
-        <v>32028</v>
+        <v>18848</v>
       </c>
       <c r="B293" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C293" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294">
-        <v>32027</v>
+        <v>18849</v>
       </c>
       <c r="B294" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C294" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295">
-        <v>32025</v>
+        <v>18850</v>
       </c>
       <c r="B295" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C295" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296">
-        <v>32026</v>
+        <v>47703</v>
       </c>
       <c r="B296" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C296" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297">
-        <v>18740</v>
-      </c>
-      <c r="B297" s="1">
+        <v>21294</v>
+      </c>
+      <c r="B297" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C297" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298">
-        <v>18742</v>
-      </c>
-      <c r="B298" s="1">
+        <v>42981</v>
+      </c>
+      <c r="B298" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C298" t="s">
-        <v>23</v>
+      <c r="C298" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D298" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299">
-        <v>18741</v>
-      </c>
-      <c r="B299" s="1">
-        <v>5</v>
-      </c>
-      <c r="C299" t="s">
-        <v>23</v>
+        <v>42982</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D299" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300">
-        <v>21176</v>
+        <v>32029</v>
       </c>
       <c r="B300" s="1">
-        <v>5</v>
-      </c>
-      <c r="C300" s="2" t="s">
-        <v>52</v>
+        <v>1</v>
+      </c>
+      <c r="C300" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301">
-        <v>47158</v>
+        <v>32028</v>
       </c>
       <c r="B301" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C301" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302">
-        <v>47159</v>
+        <v>32027</v>
       </c>
       <c r="B302" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C302" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303">
-        <v>47160</v>
+        <v>32025</v>
       </c>
       <c r="B303" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C303" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304">
-        <v>47161</v>
+        <v>32026</v>
       </c>
       <c r="B304" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C304" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305">
-        <v>47162</v>
+        <v>18740</v>
       </c>
       <c r="B305" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C305" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306">
-        <v>47163</v>
+        <v>18742</v>
       </c>
       <c r="B306" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C306" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307">
-        <v>47164</v>
+        <v>18741</v>
       </c>
       <c r="B307" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C307" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308">
-        <v>47165</v>
+        <v>21176</v>
       </c>
       <c r="B308" s="1">
-        <v>8</v>
-      </c>
-      <c r="C308" t="s">
-        <v>82</v>
+        <v>5</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309">
-        <v>47166</v>
+        <v>47158</v>
       </c>
       <c r="B309" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C309" t="s">
         <v>82</v>
@@ -4672,10 +4709,10 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310">
-        <v>47167</v>
+        <v>47159</v>
       </c>
       <c r="B310" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C310" t="s">
         <v>82</v>
@@ -4683,208 +4720,208 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311">
-        <v>12964</v>
-      </c>
-      <c r="B311" s="1" t="s">
-        <v>0</v>
+        <v>47160</v>
+      </c>
+      <c r="B311" s="1">
+        <v>3</v>
       </c>
       <c r="C311" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312">
-        <v>19803</v>
-      </c>
-      <c r="B312" s="1" t="s">
-        <v>2</v>
+        <v>47161</v>
+      </c>
+      <c r="B312" s="1">
+        <v>4</v>
       </c>
       <c r="C312" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313">
-        <v>19804</v>
-      </c>
-      <c r="B313" s="1" t="s">
-        <v>3</v>
+        <v>47162</v>
+      </c>
+      <c r="B313" s="1">
+        <v>5</v>
       </c>
       <c r="C313" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314">
-        <v>19805</v>
-      </c>
-      <c r="B314" s="1" t="s">
-        <v>4</v>
+        <v>47163</v>
+      </c>
+      <c r="B314" s="1">
+        <v>6</v>
       </c>
       <c r="C314" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315">
-        <v>19800</v>
-      </c>
-      <c r="B315" s="1" t="s">
-        <v>1</v>
+        <v>47164</v>
+      </c>
+      <c r="B315" s="1">
+        <v>7</v>
       </c>
       <c r="C315" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316">
-        <v>18864</v>
+        <v>47165</v>
       </c>
       <c r="B316" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C316" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317">
-        <v>18865</v>
+        <v>47166</v>
       </c>
       <c r="B317" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C317" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318">
-        <v>19228</v>
+        <v>47167</v>
       </c>
       <c r="B318" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C318" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319">
-        <v>19229</v>
-      </c>
-      <c r="B319" s="1">
-        <v>4</v>
+        <v>12964</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C319" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320">
-        <v>19230</v>
-      </c>
-      <c r="B320" s="1">
-        <v>5</v>
-      </c>
-      <c r="C320" s="2" t="s">
-        <v>27</v>
+        <v>19803</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C320" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321">
-        <v>19231</v>
-      </c>
-      <c r="B321" s="1">
-        <v>6</v>
+        <v>19804</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C321" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322">
-        <v>21256</v>
-      </c>
-      <c r="B322" s="1">
-        <v>1</v>
+        <v>19805</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C322" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323">
-        <v>21257</v>
-      </c>
-      <c r="B323" s="1">
-        <v>2</v>
+        <v>19800</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C323" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324">
-        <v>21260</v>
-      </c>
-      <c r="B324" s="1">
-        <v>3</v>
+        <v>19231</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C324" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325">
-        <v>21261</v>
-      </c>
-      <c r="B325" s="1">
-        <v>4</v>
+        <v>18864</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C325" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326">
-        <v>21269</v>
-      </c>
-      <c r="B326" s="1">
-        <v>5</v>
+        <v>18865</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C326" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327">
-        <v>21270</v>
-      </c>
-      <c r="B327" s="1">
-        <v>6</v>
+        <v>19228</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C327" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328">
-        <v>47252</v>
-      </c>
-      <c r="B328" s="1">
-        <v>8</v>
+        <v>19229</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C328" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329">
-        <v>49468</v>
+        <v>21256</v>
       </c>
       <c r="B329" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C329" t="s">
         <v>43</v>
@@ -4892,10 +4929,10 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330">
-        <v>21318</v>
+        <v>21257</v>
       </c>
       <c r="B330" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C330" t="s">
         <v>43</v>
@@ -4903,10 +4940,10 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331">
-        <v>21005</v>
+        <v>21260</v>
       </c>
       <c r="B331" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C331" t="s">
         <v>43</v>
@@ -4914,87 +4951,87 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332">
-        <v>46393</v>
+        <v>21261</v>
       </c>
       <c r="B332" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C332" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333">
-        <v>46395</v>
+        <v>21269</v>
       </c>
       <c r="B333" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C333" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334">
-        <v>46396</v>
+        <v>21270</v>
       </c>
       <c r="B334" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C334" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335">
-        <v>46394</v>
+        <v>47252</v>
       </c>
       <c r="B335" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C335" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336">
-        <v>46398</v>
+        <v>49468</v>
       </c>
       <c r="B336" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C336" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337">
-        <v>46399</v>
+        <v>21318</v>
       </c>
       <c r="B337" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C337" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338">
-        <v>46397</v>
+        <v>21005</v>
       </c>
       <c r="B338" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C338" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339">
-        <v>51199</v>
+        <v>46393</v>
       </c>
       <c r="B339" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C339" t="s">
         <v>79</v>
@@ -5002,10 +5039,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340">
-        <v>46401</v>
+        <v>46395</v>
       </c>
       <c r="B340" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C340" t="s">
         <v>79</v>
@@ -5013,10 +5050,10 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341">
-        <v>46402</v>
+        <v>46396</v>
       </c>
       <c r="B341" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C341" t="s">
         <v>79</v>
@@ -5024,10 +5061,10 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342">
-        <v>46403</v>
+        <v>46394</v>
       </c>
       <c r="B342" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C342" t="s">
         <v>79</v>
@@ -5035,464 +5072,464 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A343">
-        <v>23175</v>
+        <v>46398</v>
       </c>
       <c r="B343" s="1">
-        <v>51</v>
-      </c>
-      <c r="C343" s="2" t="s">
-        <v>96</v>
+        <v>6</v>
+      </c>
+      <c r="C343" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A344">
-        <v>23176</v>
+        <v>46399</v>
       </c>
       <c r="B344" s="1">
-        <v>74</v>
-      </c>
-      <c r="C344" s="2" t="s">
-        <v>96</v>
+        <v>7</v>
+      </c>
+      <c r="C344" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345">
-        <v>23183</v>
+        <v>46397</v>
       </c>
       <c r="B345" s="1">
-        <v>74</v>
-      </c>
-      <c r="C345" s="2" t="s">
-        <v>96</v>
+        <v>8</v>
+      </c>
+      <c r="C345" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346">
-        <v>23173</v>
+        <v>51199</v>
       </c>
       <c r="B346" s="1">
-        <v>75</v>
-      </c>
-      <c r="C346" s="2" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="C346" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347">
-        <v>20983</v>
+        <v>46401</v>
       </c>
       <c r="B347" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C347" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348">
-        <v>20984</v>
+        <v>46402</v>
       </c>
       <c r="B348" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C348" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349">
-        <v>20985</v>
+        <v>46403</v>
       </c>
       <c r="B349" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C349" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350">
-        <v>20986</v>
+        <v>23175</v>
       </c>
       <c r="B350" s="1">
-        <v>4</v>
-      </c>
-      <c r="C350" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="C350" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351">
-        <v>20987</v>
+        <v>23176</v>
       </c>
       <c r="B351" s="1">
-        <v>5</v>
-      </c>
-      <c r="C351" t="s">
-        <v>41</v>
+        <v>74</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352">
-        <v>20988</v>
+        <v>23183</v>
       </c>
       <c r="B352" s="1">
-        <v>6</v>
-      </c>
-      <c r="C352" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353">
-        <v>20989</v>
+        <v>23173</v>
       </c>
       <c r="B353" s="1">
-        <v>7</v>
-      </c>
-      <c r="C353" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="C353" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354">
-        <v>20990</v>
+        <v>20983</v>
       </c>
       <c r="B354" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C354" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355">
-        <v>20991</v>
+        <v>20984</v>
       </c>
       <c r="B355" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C355" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356">
+        <v>20985</v>
+      </c>
+      <c r="B356" s="1">
+        <v>3</v>
+      </c>
+      <c r="C356" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A357">
+        <v>20986</v>
+      </c>
+      <c r="B357" s="1">
+        <v>4</v>
+      </c>
+      <c r="C357" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A358">
+        <v>20987</v>
+      </c>
+      <c r="B358" s="1">
+        <v>5</v>
+      </c>
+      <c r="C358" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A359">
+        <v>20988</v>
+      </c>
+      <c r="B359" s="1">
+        <v>6</v>
+      </c>
+      <c r="C359" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A360">
+        <v>20989</v>
+      </c>
+      <c r="B360" s="1">
+        <v>7</v>
+      </c>
+      <c r="C360" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A361">
+        <v>20990</v>
+      </c>
+      <c r="B361" s="1">
+        <v>8</v>
+      </c>
+      <c r="C361" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A362">
+        <v>20991</v>
+      </c>
+      <c r="B362" s="1">
+        <v>9</v>
+      </c>
+      <c r="C362" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A363">
         <v>41461</v>
       </c>
-      <c r="B356" s="1">
+      <c r="B363" s="1">
         <v>1</v>
       </c>
-      <c r="C356" s="2" t="s">
+      <c r="C363" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A357">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A364">
         <v>41462</v>
       </c>
-      <c r="B357" s="1">
+      <c r="B364" s="1">
         <v>2</v>
       </c>
-      <c r="C357" s="2" t="s">
+      <c r="C364" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A358">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A365">
         <v>41463</v>
       </c>
-      <c r="B358" s="1">
+      <c r="B365" s="1">
         <v>3</v>
       </c>
-      <c r="C358" s="2" t="s">
+      <c r="C365" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A359">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A366">
         <v>41464</v>
       </c>
-      <c r="B359" s="1">
+      <c r="B366" s="1">
         <v>4</v>
       </c>
-      <c r="C359" s="2" t="s">
+      <c r="C366" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A360">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A367">
         <v>41465</v>
       </c>
-      <c r="B360" s="1">
+      <c r="B367" s="1">
         <v>5</v>
       </c>
-      <c r="C360" s="2" t="s">
+      <c r="C367" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A361">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A368">
         <v>41466</v>
       </c>
-      <c r="B361" s="1">
+      <c r="B368" s="1">
         <v>6</v>
       </c>
-      <c r="C361" s="2" t="s">
+      <c r="C368" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A362">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A369">
         <v>21314</v>
       </c>
-      <c r="B362" s="1">
+      <c r="B369" s="1">
         <v>1</v>
       </c>
-      <c r="C362" t="s">
+      <c r="C369" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A363">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A370">
         <v>21315</v>
       </c>
-      <c r="B363" s="1">
+      <c r="B370" s="1">
         <v>2</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C370" t="s">
         <v>59</v>
       </c>
-      <c r="D363" t="s">
+      <c r="D370" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A364">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A371">
         <v>21316</v>
       </c>
-      <c r="B364" s="1">
+      <c r="B371" s="1">
         <v>3</v>
       </c>
-      <c r="C364" t="s">
+      <c r="C371" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A365">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A372">
         <v>20816</v>
-      </c>
-      <c r="B365" s="1">
-        <v>1</v>
-      </c>
-      <c r="C365" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A366">
-        <v>18754</v>
-      </c>
-      <c r="B366" s="1">
-        <v>2</v>
-      </c>
-      <c r="C366" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A367">
-        <v>18755</v>
-      </c>
-      <c r="B367" s="1">
-        <v>3</v>
-      </c>
-      <c r="C367" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A368">
-        <v>18758</v>
-      </c>
-      <c r="B368" s="1">
-        <v>4</v>
-      </c>
-      <c r="C368" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A369">
-        <v>22341</v>
-      </c>
-      <c r="B369" s="1">
-        <v>5</v>
-      </c>
-      <c r="C369" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A370">
-        <v>18759</v>
-      </c>
-      <c r="B370" s="1">
-        <v>6</v>
-      </c>
-      <c r="C370" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A371">
-        <v>18760</v>
-      </c>
-      <c r="B371" s="1">
-        <v>7</v>
-      </c>
-      <c r="C371" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A372">
-        <v>18765</v>
       </c>
       <c r="B372" s="1">
         <v>1</v>
       </c>
       <c r="C372" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A373">
-        <v>18750</v>
+        <v>18754</v>
       </c>
       <c r="B373" s="1">
         <v>2</v>
       </c>
       <c r="C373" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A374">
-        <v>40947</v>
+        <v>18755</v>
       </c>
       <c r="B374" s="1">
         <v>3</v>
       </c>
       <c r="C374" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A375">
-        <v>40946</v>
+        <v>18758</v>
       </c>
       <c r="B375" s="1">
         <v>4</v>
       </c>
       <c r="C375" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A376">
-        <v>18749</v>
+        <v>22341</v>
       </c>
       <c r="B376" s="1">
         <v>5</v>
       </c>
       <c r="C376" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A377">
-        <v>18766</v>
+        <v>18759</v>
       </c>
       <c r="B377" s="1">
         <v>6</v>
       </c>
       <c r="C377" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A378">
-        <v>18761</v>
+        <v>18760</v>
       </c>
       <c r="B378" s="1">
         <v>7</v>
       </c>
       <c r="C378" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A379">
-        <v>18752</v>
+        <v>18765</v>
       </c>
       <c r="B379" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C379" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A380">
-        <v>18751</v>
+        <v>18750</v>
       </c>
       <c r="B380" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C380" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A381">
-        <v>18763</v>
+        <v>40947</v>
       </c>
       <c r="B381" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C381" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A382">
-        <v>18762</v>
+        <v>40946</v>
       </c>
       <c r="B382" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C382" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A383">
-        <v>18764</v>
+        <v>18749</v>
       </c>
       <c r="B383" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C383" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A384">
-        <v>22342</v>
+        <v>18766</v>
       </c>
       <c r="B384" s="1">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C384" t="s">
         <v>24</v>
@@ -5500,405 +5537,479 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A385">
-        <v>50255</v>
+        <v>18761</v>
       </c>
       <c r="B385" s="1">
-        <v>1</v>
-      </c>
-      <c r="C385" s="2" t="s">
-        <v>97</v>
+        <v>7</v>
+      </c>
+      <c r="C385" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A386">
-        <v>50256</v>
+        <v>18752</v>
       </c>
       <c r="B386" s="1">
-        <v>2</v>
-      </c>
-      <c r="C386" s="2" t="s">
-        <v>97</v>
+        <v>8</v>
+      </c>
+      <c r="C386" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A387">
-        <v>50257</v>
+        <v>18751</v>
       </c>
       <c r="B387" s="1">
-        <v>3</v>
-      </c>
-      <c r="C387" s="2" t="s">
-        <v>97</v>
+        <v>9</v>
+      </c>
+      <c r="C387" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A388">
-        <v>50258</v>
+        <v>18763</v>
       </c>
       <c r="B388" s="1">
-        <v>4</v>
-      </c>
-      <c r="C388" s="2" t="s">
-        <v>97</v>
+        <v>10</v>
+      </c>
+      <c r="C388" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A389">
-        <v>50259</v>
+        <v>18762</v>
       </c>
       <c r="B389" s="1">
-        <v>5</v>
-      </c>
-      <c r="C389" s="2" t="s">
-        <v>97</v>
+        <v>11</v>
+      </c>
+      <c r="C389" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A390">
-        <v>50260</v>
+        <v>18764</v>
       </c>
       <c r="B390" s="1">
-        <v>6</v>
-      </c>
-      <c r="C390" s="2" t="s">
-        <v>97</v>
+        <v>12</v>
+      </c>
+      <c r="C390" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A391">
-        <v>19555</v>
+        <v>22342</v>
       </c>
       <c r="B391" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C391" t="s">
-        <v>29</v>
-      </c>
-      <c r="D391" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A392">
-        <v>21129</v>
+        <v>50255</v>
       </c>
       <c r="B392" s="1">
         <v>1</v>
       </c>
-      <c r="C392" t="s">
-        <v>47</v>
+      <c r="C392" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A393">
-        <v>21128</v>
+        <v>50256</v>
       </c>
       <c r="B393" s="1">
         <v>2</v>
       </c>
-      <c r="C393" t="s">
-        <v>47</v>
+      <c r="C393" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A394">
-        <v>40693</v>
+        <v>50257</v>
       </c>
       <c r="B394" s="1">
         <v>3</v>
       </c>
-      <c r="C394" t="s">
-        <v>47</v>
+      <c r="C394" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A395">
-        <v>21130</v>
+        <v>50258</v>
       </c>
       <c r="B395" s="1">
         <v>4</v>
       </c>
-      <c r="C395" t="s">
-        <v>47</v>
+      <c r="C395" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A396">
-        <v>23278</v>
+        <v>50259</v>
       </c>
       <c r="B396" s="1">
         <v>5</v>
       </c>
-      <c r="C396" t="s">
-        <v>47</v>
+      <c r="C396" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A397">
-        <v>23418</v>
+        <v>50260</v>
       </c>
       <c r="B397" s="1">
         <v>6</v>
       </c>
-      <c r="C397" t="s">
-        <v>47</v>
+      <c r="C397" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A398">
-        <v>47644</v>
+        <v>19555</v>
       </c>
       <c r="B398" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C398" t="s">
-        <v>47</v>
+        <v>29</v>
+      </c>
+      <c r="D398" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A399">
-        <v>20965</v>
-      </c>
-      <c r="B399" s="1">
-        <v>1</v>
+        <v>47668</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C399" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A400">
-        <v>20972</v>
-      </c>
-      <c r="B400" s="1">
-        <v>2</v>
+        <v>47669</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C400" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401">
-        <v>20970</v>
-      </c>
-      <c r="B401" s="1">
-        <v>3</v>
+        <v>47670</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C401" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402">
-        <v>20968</v>
+        <v>21129</v>
       </c>
       <c r="B402" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C402" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403">
-        <v>20967</v>
+        <v>21128</v>
       </c>
       <c r="B403" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C403" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404">
-        <v>20971</v>
+        <v>40693</v>
       </c>
       <c r="B404" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C404" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405">
-        <v>44766</v>
+        <v>21130</v>
       </c>
       <c r="B405" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C405" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406">
-        <v>46697</v>
+        <v>23278</v>
       </c>
       <c r="B406" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C406" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407">
-        <v>46696</v>
+        <v>23418</v>
       </c>
       <c r="B407" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C407" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408">
-        <v>46698</v>
+        <v>47644</v>
       </c>
       <c r="B408" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C408" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409">
-        <v>46700</v>
+        <v>20965</v>
       </c>
       <c r="B409" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C409" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A410">
-        <v>46701</v>
+        <v>20972</v>
       </c>
       <c r="B410" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C410" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411">
-        <v>50261</v>
+        <v>20970</v>
       </c>
       <c r="B411" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C411" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412">
-        <v>50262</v>
+        <v>20968</v>
       </c>
       <c r="B412" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C412" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413">
-        <v>50263</v>
+        <v>20967</v>
       </c>
       <c r="B413" s="1">
-        <v>3</v>
-      </c>
-      <c r="C413" s="2" t="s">
-        <v>89</v>
+        <v>5</v>
+      </c>
+      <c r="C413" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414">
-        <v>50265</v>
+        <v>20971</v>
       </c>
       <c r="B414" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C414" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415">
-        <v>50266</v>
+        <v>44766</v>
       </c>
       <c r="B415" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C415" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416">
-        <v>50267</v>
+        <v>46697</v>
       </c>
       <c r="B416" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C416" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417">
-        <v>47668</v>
-      </c>
-      <c r="B417" s="1" t="s">
-        <v>105</v>
+        <v>46696</v>
+      </c>
+      <c r="B417" s="1">
+        <v>2</v>
       </c>
       <c r="C417" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418">
-        <v>47669</v>
-      </c>
-      <c r="B418" s="1" t="s">
-        <v>106</v>
+        <v>46698</v>
+      </c>
+      <c r="B418" s="1">
+        <v>3</v>
       </c>
       <c r="C418" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419">
-        <v>47670</v>
-      </c>
-      <c r="B419" s="1" t="s">
-        <v>107</v>
+        <v>46700</v>
+      </c>
+      <c r="B419" s="1">
+        <v>4</v>
       </c>
       <c r="C419" t="s">
-        <v>108</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <v>46701</v>
+      </c>
+      <c r="B420" s="1">
+        <v>5</v>
+      </c>
+      <c r="C420" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <v>50261</v>
+      </c>
+      <c r="B421" s="1">
+        <v>1</v>
+      </c>
+      <c r="C421" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <v>50262</v>
+      </c>
+      <c r="B422" s="1">
+        <v>2</v>
+      </c>
+      <c r="C422" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <v>50263</v>
+      </c>
+      <c r="B423" s="1">
+        <v>3</v>
+      </c>
+      <c r="C423" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <v>50265</v>
+      </c>
+      <c r="B424" s="1">
+        <v>5</v>
+      </c>
+      <c r="C424" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>50266</v>
+      </c>
+      <c r="B425" s="1">
+        <v>6</v>
+      </c>
+      <c r="C425" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>50267</v>
+      </c>
+      <c r="B426" s="1">
+        <v>7</v>
+      </c>
+      <c r="C426" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C416" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C416">
-      <sortCondition ref="C1:C416"/>
+  <autoFilter ref="A1:C415" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C415">
+      <sortCondition ref="C1:C415"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D416">
-    <sortCondition ref="C2:C416"/>
-    <sortCondition ref="B2:B416"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D426">
+    <sortCondition ref="C2:C426"/>
+    <sortCondition ref="B2:B426"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <ignoredErrors>
-    <ignoredError sqref="B417:B419" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update sale operator & knox city sc bus bays
</commit_message>
<xml_diff>
--- a/excel/bus/bays/Bus Bays.xlsx
+++ b/excel/bus/bays/Bus Bays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardyeung/Projects/TVData/excel/bus/bays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F2824C-BF8C-104B-AA34-7462A6FB1FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C35FFD4-E555-CE43-B9BB-A8949176EADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F3FC56B-3071-1747-8E11-6356A10C0FCD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="130">
   <si>
     <t>E</t>
   </si>
@@ -393,6 +393,39 @@
   </si>
   <si>
     <t>PTV also has the bays wrong, showing 51389 as B and 27854 as C</t>
+  </si>
+  <si>
+    <t>TRBS and coach stop</t>
+  </si>
+  <si>
+    <t>Former Bay 1</t>
+  </si>
+  <si>
+    <t>Former Bay 2</t>
+  </si>
+  <si>
+    <t>Former Bay 3</t>
+  </si>
+  <si>
+    <t>Former Bay 4</t>
+  </si>
+  <si>
+    <t>Former Bay 5</t>
+  </si>
+  <si>
+    <t>Former Bay 6</t>
+  </si>
+  <si>
+    <t>Former Bay 7</t>
+  </si>
+  <si>
+    <t>Former Bay 8</t>
+  </si>
+  <si>
+    <t>Former Bay 9</t>
+  </si>
+  <si>
+    <t>Former Bay 10</t>
   </si>
 </sst>
 </file>
@@ -1265,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
   <dimension ref="A1:D425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="141" workbookViewId="0">
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2524,7 +2557,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>45538</v>
       </c>
@@ -2535,7 +2568,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>19822</v>
       </c>
@@ -2546,7 +2579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>1612</v>
       </c>
@@ -2557,7 +2590,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>19824</v>
       </c>
@@ -2568,7 +2601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>4251</v>
       </c>
@@ -2579,7 +2612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>20157</v>
       </c>
@@ -2590,7 +2623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>21326</v>
       </c>
@@ -2601,7 +2634,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>19817</v>
       </c>
@@ -2612,7 +2645,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>51295</v>
       </c>
@@ -2623,7 +2656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>20018</v>
       </c>
@@ -2633,8 +2666,11 @@
       <c r="C122" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>22250</v>
       </c>
@@ -2645,7 +2681,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>51132</v>
       </c>
@@ -2656,7 +2692,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>51133</v>
       </c>
@@ -2667,7 +2703,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>51134</v>
       </c>
@@ -2678,7 +2714,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>19474</v>
       </c>
@@ -2689,7 +2725,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>19483</v>
       </c>
@@ -3598,110 +3634,140 @@
       <c r="A210">
         <v>40359</v>
       </c>
-      <c r="B210" s="1">
+      <c r="B210" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C210" t="s">
         <v>31</v>
+      </c>
+      <c r="D210" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>19637</v>
       </c>
-      <c r="B211" s="1">
-        <v>2</v>
+      <c r="B211" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C211" t="s">
         <v>31</v>
+      </c>
+      <c r="D211" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>19636</v>
       </c>
-      <c r="B212" s="1">
-        <v>3</v>
+      <c r="B212" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C212" t="s">
         <v>31</v>
+      </c>
+      <c r="D212" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>19635</v>
       </c>
-      <c r="B213" s="1">
-        <v>4</v>
+      <c r="B213" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C213" t="s">
         <v>31</v>
+      </c>
+      <c r="D213" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>19634</v>
       </c>
-      <c r="B214" s="1">
-        <v>5</v>
+      <c r="B214" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C214" t="s">
         <v>31</v>
+      </c>
+      <c r="D214" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>40358</v>
       </c>
-      <c r="B215" s="1">
-        <v>6</v>
+      <c r="B215" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C215" t="s">
         <v>31</v>
+      </c>
+      <c r="D215" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>19632</v>
       </c>
-      <c r="B216" s="1">
-        <v>7</v>
+      <c r="B216" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C216" t="s">
         <v>31</v>
+      </c>
+      <c r="D216" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>19631</v>
       </c>
-      <c r="B217" s="1">
-        <v>8</v>
+      <c r="B217" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C217" t="s">
         <v>31</v>
+      </c>
+      <c r="D217" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>19630</v>
       </c>
-      <c r="B218" s="1">
-        <v>9</v>
+      <c r="B218" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C218" t="s">
         <v>31</v>
+      </c>
+      <c r="D218" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>19629</v>
       </c>
-      <c r="B219" s="1">
-        <v>10</v>
+      <c r="B219" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C219" t="s">
         <v>31</v>
+      </c>
+      <c r="D219" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
remove skybus city shuttle stop and update test
</commit_message>
<xml_diff>
--- a/excel/bus/bays/Bus Bays.xlsx
+++ b/excel/bus/bays/Bus Bays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardyeung/Projects/TVData/excel/bus/bays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C35FFD4-E555-CE43-B9BB-A8949176EADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE36B86-D2B7-EC43-A92D-294CC5C6BC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F3FC56B-3071-1747-8E11-6356A10C0FCD}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="bays" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bays!$A$1:$C$414</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bays!$A$1:$C$413</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="131">
   <si>
     <t>E</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>Former Bay 10</t>
+  </si>
+  <si>
+    <t>Skybus arrivals</t>
   </si>
 </sst>
 </file>
@@ -1296,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
-  <dimension ref="A1:D425"/>
+  <dimension ref="A1:D424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="141" workbookViewId="0">
-      <selection activeCell="B219" sqref="B219"/>
+    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C350" sqref="C350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5081,7 +5084,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>21005</v>
       </c>
@@ -5092,7 +5095,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>46393</v>
       </c>
@@ -5103,7 +5106,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>46395</v>
       </c>
@@ -5114,7 +5117,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>46396</v>
       </c>
@@ -5125,7 +5128,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>46394</v>
       </c>
@@ -5136,7 +5139,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>46398</v>
       </c>
@@ -5147,7 +5150,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>46399</v>
       </c>
@@ -5158,7 +5161,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>46397</v>
       </c>
@@ -5169,7 +5172,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>51199</v>
       </c>
@@ -5180,7 +5183,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>46401</v>
       </c>
@@ -5191,7 +5194,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>46402</v>
       </c>
@@ -5202,7 +5205,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>46403</v>
       </c>
@@ -5213,7 +5216,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>23175</v>
       </c>
@@ -5223,10 +5226,13 @@
       <c r="C349" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D349" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A350">
-        <v>23176</v>
+        <v>23183</v>
       </c>
       <c r="B350" s="1">
         <v>74</v>
@@ -5235,378 +5241,378 @@
         <v>96</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A351">
-        <v>23183</v>
+        <v>23173</v>
       </c>
       <c r="B351" s="1">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A352">
-        <v>23173</v>
+        <v>20983</v>
       </c>
       <c r="B352" s="1">
-        <v>75</v>
-      </c>
-      <c r="C352" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C352" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A353">
-        <v>20983</v>
+        <v>20984</v>
       </c>
       <c r="B353" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C353" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A354">
-        <v>20984</v>
+        <v>20985</v>
       </c>
       <c r="B354" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C354" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A355">
-        <v>20985</v>
+        <v>20986</v>
       </c>
       <c r="B355" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C355" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A356">
-        <v>20986</v>
+        <v>20987</v>
       </c>
       <c r="B356" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C356" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357">
-        <v>20987</v>
+        <v>20988</v>
       </c>
       <c r="B357" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C357" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358">
-        <v>20988</v>
+        <v>20989</v>
       </c>
       <c r="B358" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C358" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A359">
-        <v>20989</v>
+        <v>20990</v>
       </c>
       <c r="B359" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C359" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A360">
-        <v>20990</v>
+        <v>20991</v>
       </c>
       <c r="B360" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C360" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361">
-        <v>20991</v>
+        <v>41461</v>
       </c>
       <c r="B361" s="1">
-        <v>9</v>
-      </c>
-      <c r="C361" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362">
-        <v>41461</v>
+        <v>41462</v>
       </c>
       <c r="B362" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363">
-        <v>41462</v>
+        <v>41463</v>
       </c>
       <c r="B363" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364">
-        <v>41463</v>
+        <v>41464</v>
       </c>
       <c r="B364" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365">
-        <v>41464</v>
+        <v>41465</v>
       </c>
       <c r="B365" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A366">
-        <v>41465</v>
+        <v>41466</v>
       </c>
       <c r="B366" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A367">
-        <v>41466</v>
+        <v>21314</v>
       </c>
       <c r="B367" s="1">
-        <v>6</v>
-      </c>
-      <c r="C367" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C367" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A368">
-        <v>21314</v>
+        <v>21315</v>
       </c>
       <c r="B368" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C368" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D368" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369">
-        <v>21315</v>
+        <v>21316</v>
       </c>
       <c r="B369" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C369" t="s">
         <v>59</v>
       </c>
-      <c r="D369" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370">
-        <v>21316</v>
+        <v>20816</v>
       </c>
       <c r="B370" s="1">
+        <v>1</v>
+      </c>
+      <c r="C370" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A371">
+        <v>18754</v>
+      </c>
+      <c r="B371" s="1">
+        <v>2</v>
+      </c>
+      <c r="C371" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A372">
+        <v>18755</v>
+      </c>
+      <c r="B372" s="1">
         <v>3</v>
-      </c>
-      <c r="C370" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A371">
-        <v>20816</v>
-      </c>
-      <c r="B371" s="1">
-        <v>1</v>
-      </c>
-      <c r="C371" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A372">
-        <v>18754</v>
-      </c>
-      <c r="B372" s="1">
-        <v>2</v>
       </c>
       <c r="C372" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373">
-        <v>18755</v>
+        <v>18758</v>
       </c>
       <c r="B373" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C373" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374">
-        <v>18758</v>
+        <v>22341</v>
       </c>
       <c r="B374" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C374" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375">
-        <v>22341</v>
+        <v>18759</v>
       </c>
       <c r="B375" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C375" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376">
-        <v>18759</v>
+        <v>18760</v>
       </c>
       <c r="B376" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C376" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377">
-        <v>18760</v>
+        <v>18765</v>
       </c>
       <c r="B377" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C377" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378">
-        <v>18765</v>
+        <v>18750</v>
       </c>
       <c r="B378" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C378" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379">
-        <v>18750</v>
+        <v>40947</v>
       </c>
       <c r="B379" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C379" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380">
-        <v>40947</v>
+        <v>40946</v>
       </c>
       <c r="B380" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C380" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381">
-        <v>40946</v>
+        <v>18749</v>
       </c>
       <c r="B381" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C381" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382">
-        <v>18749</v>
+        <v>18766</v>
       </c>
       <c r="B382" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C382" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383">
-        <v>18766</v>
+        <v>18761</v>
       </c>
       <c r="B383" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C383" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384">
-        <v>18761</v>
+        <v>18752</v>
       </c>
       <c r="B384" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C384" t="s">
         <v>24</v>
@@ -5614,10 +5620,10 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A385">
-        <v>18752</v>
+        <v>18751</v>
       </c>
       <c r="B385" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C385" t="s">
         <v>24</v>
@@ -5625,10 +5631,10 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A386">
-        <v>18751</v>
+        <v>18763</v>
       </c>
       <c r="B386" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C386" t="s">
         <v>24</v>
@@ -5636,10 +5642,10 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A387">
-        <v>18763</v>
+        <v>18762</v>
       </c>
       <c r="B387" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C387" t="s">
         <v>24</v>
@@ -5647,10 +5653,10 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A388">
-        <v>18762</v>
+        <v>18764</v>
       </c>
       <c r="B388" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C388" t="s">
         <v>24</v>
@@ -5658,10 +5664,10 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A389">
-        <v>18764</v>
+        <v>22342</v>
       </c>
       <c r="B389" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C389" t="s">
         <v>24</v>
@@ -5669,21 +5675,21 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A390">
-        <v>22342</v>
+        <v>50255</v>
       </c>
       <c r="B390" s="1">
-        <v>13</v>
-      </c>
-      <c r="C390" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A391">
-        <v>50255</v>
+        <v>50256</v>
       </c>
       <c r="B391" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C391" s="2" t="s">
         <v>97</v>
@@ -5691,10 +5697,10 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A392">
-        <v>50256</v>
+        <v>50257</v>
       </c>
       <c r="B392" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C392" s="2" t="s">
         <v>97</v>
@@ -5702,10 +5708,10 @@
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A393">
-        <v>50257</v>
+        <v>50258</v>
       </c>
       <c r="B393" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>97</v>
@@ -5713,10 +5719,10 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A394">
-        <v>50258</v>
+        <v>50259</v>
       </c>
       <c r="B394" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C394" s="2" t="s">
         <v>97</v>
@@ -5724,10 +5730,10 @@
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A395">
-        <v>50259</v>
+        <v>50260</v>
       </c>
       <c r="B395" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>97</v>
@@ -5735,35 +5741,35 @@
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A396">
-        <v>50260</v>
+        <v>19555</v>
       </c>
       <c r="B396" s="1">
-        <v>6</v>
-      </c>
-      <c r="C396" s="2" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="C396" t="s">
+        <v>29</v>
+      </c>
+      <c r="D396" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A397">
-        <v>19555</v>
-      </c>
-      <c r="B397" s="1">
-        <v>2</v>
+        <v>47668</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C397" t="s">
-        <v>29</v>
-      </c>
-      <c r="D397" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A398">
-        <v>47668</v>
+        <v>47669</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C398" t="s">
         <v>108</v>
@@ -5771,10 +5777,10 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A399">
-        <v>47669</v>
+        <v>47670</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C399" t="s">
         <v>108</v>
@@ -5782,21 +5788,21 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A400">
-        <v>47670</v>
-      </c>
-      <c r="B400" s="1" t="s">
-        <v>107</v>
+        <v>21129</v>
+      </c>
+      <c r="B400" s="1">
+        <v>1</v>
       </c>
       <c r="C400" t="s">
-        <v>108</v>
+        <v>47</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401">
-        <v>21129</v>
+        <v>21128</v>
       </c>
       <c r="B401" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C401" t="s">
         <v>47</v>
@@ -5804,10 +5810,10 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402">
-        <v>21128</v>
+        <v>40693</v>
       </c>
       <c r="B402" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C402" t="s">
         <v>47</v>
@@ -5815,10 +5821,10 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403">
-        <v>40693</v>
+        <v>21130</v>
       </c>
       <c r="B403" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C403" t="s">
         <v>47</v>
@@ -5826,10 +5832,10 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404">
-        <v>21130</v>
+        <v>23278</v>
       </c>
       <c r="B404" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C404" t="s">
         <v>47</v>
@@ -5837,10 +5843,10 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405">
-        <v>23278</v>
+        <v>23418</v>
       </c>
       <c r="B405" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C405" t="s">
         <v>47</v>
@@ -5848,10 +5854,10 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406">
-        <v>23418</v>
+        <v>47644</v>
       </c>
       <c r="B406" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C406" t="s">
         <v>47</v>
@@ -5859,21 +5865,21 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407">
-        <v>47644</v>
+        <v>20965</v>
       </c>
       <c r="B407" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C407" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408">
-        <v>20965</v>
+        <v>20972</v>
       </c>
       <c r="B408" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C408" t="s">
         <v>40</v>
@@ -5881,10 +5887,10 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409">
-        <v>20972</v>
+        <v>20970</v>
       </c>
       <c r="B409" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C409" t="s">
         <v>40</v>
@@ -5892,10 +5898,10 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A410">
-        <v>20970</v>
+        <v>20968</v>
       </c>
       <c r="B410" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C410" t="s">
         <v>40</v>
@@ -5903,10 +5909,10 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411">
-        <v>20968</v>
+        <v>20967</v>
       </c>
       <c r="B411" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C411" t="s">
         <v>40</v>
@@ -5914,10 +5920,10 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412">
-        <v>20967</v>
+        <v>20971</v>
       </c>
       <c r="B412" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C412" t="s">
         <v>40</v>
@@ -5925,10 +5931,10 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413">
-        <v>20971</v>
+        <v>44766</v>
       </c>
       <c r="B413" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C413" t="s">
         <v>40</v>
@@ -5936,21 +5942,21 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414">
-        <v>44766</v>
+        <v>46697</v>
       </c>
       <c r="B414" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C414" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415">
-        <v>46697</v>
+        <v>46696</v>
       </c>
       <c r="B415" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C415" t="s">
         <v>80</v>
@@ -5958,10 +5964,10 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416">
-        <v>46696</v>
+        <v>46698</v>
       </c>
       <c r="B416" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C416" t="s">
         <v>80</v>
@@ -5969,10 +5975,10 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417">
-        <v>46698</v>
+        <v>46700</v>
       </c>
       <c r="B417" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C417" t="s">
         <v>80</v>
@@ -5980,10 +5986,10 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418">
-        <v>46700</v>
+        <v>46701</v>
       </c>
       <c r="B418" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C418" t="s">
         <v>80</v>
@@ -5991,21 +5997,21 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419">
-        <v>46701</v>
+        <v>50261</v>
       </c>
       <c r="B419" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C419" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420">
-        <v>50261</v>
+        <v>50262</v>
       </c>
       <c r="B420" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C420" t="s">
         <v>89</v>
@@ -6013,32 +6019,32 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421">
-        <v>50262</v>
+        <v>50263</v>
       </c>
       <c r="B421" s="1">
-        <v>2</v>
-      </c>
-      <c r="C421" t="s">
+        <v>3</v>
+      </c>
+      <c r="C421" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422">
-        <v>50263</v>
+        <v>50265</v>
       </c>
       <c r="B422" s="1">
-        <v>3</v>
-      </c>
-      <c r="C422" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C422" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423">
-        <v>50265</v>
+        <v>50266</v>
       </c>
       <c r="B423" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C423" t="s">
         <v>89</v>
@@ -6046,35 +6052,24 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424">
-        <v>50266</v>
+        <v>50267</v>
       </c>
       <c r="B424" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C424" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A425">
-        <v>50267</v>
-      </c>
-      <c r="B425" s="1">
-        <v>7</v>
-      </c>
-      <c r="C425" t="s">
-        <v>89</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C414" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C414">
-      <sortCondition ref="C1:C414"/>
+  <autoFilter ref="A1:C413" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C413">
+      <sortCondition ref="C1:C413"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D425">
-    <sortCondition ref="C2:C425"/>
-    <sortCondition ref="B2:B425"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D424">
+    <sortCondition ref="C2:C424"/>
+    <sortCondition ref="B2:B424"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add in Melb Uni, Pacific Werribee, Tarneit & Update Wyndham Vale & Laverton
</commit_message>
<xml_diff>
--- a/excel/bus/bays/Bus Bays.xlsx
+++ b/excel/bus/bays/Bus Bays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardyeung/Projects/TVData/excel/bus/bays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE36B86-D2B7-EC43-A92D-294CC5C6BC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F190F30D-2CCC-A143-A69D-42BE8E24C684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F3FC56B-3071-1747-8E11-6356A10C0FCD}"/>
   </bookViews>
@@ -16,9 +16,10 @@
     <sheet name="bays" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bays!$A$1:$C$413</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bays!$A$1:$C$416</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="141">
   <si>
     <t>E</t>
   </si>
@@ -429,13 +430,43 @@
   </si>
   <si>
     <t>Skybus arrivals</t>
+  </si>
+  <si>
+    <t>Hampton Station/Willis Lane (Hampton)</t>
+  </si>
+  <si>
+    <t>Melbourne University/Grattan St (Carlton)</t>
+  </si>
+  <si>
+    <t>no bay A? (possibly 28672)</t>
+  </si>
+  <si>
+    <t>Werribee Plaza/Derrimut Rd (Hoppers Crossing)</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>TRBS stop, 4 unused</t>
+  </si>
+  <si>
+    <t>Tarneit Station (Tarneit)</t>
+  </si>
+  <si>
+    <t>new interchange</t>
+  </si>
+  <si>
+    <t>Bay E used for layover, no gap in stop ID for this</t>
+  </si>
+  <si>
+    <t>Removed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -566,6 +597,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -918,12 +955,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1299,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
-  <dimension ref="A1:D424"/>
+  <dimension ref="A1:D450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C350" sqref="C350"/>
+    <sheetView tabSelected="1" topLeftCell="A215" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C207" sqref="C207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3446,177 +3487,180 @@
         <v>44</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193">
+        <v>20767</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C193" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>3587</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C194" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195">
         <v>51735</v>
-      </c>
-      <c r="B193" s="1">
-        <v>1</v>
-      </c>
-      <c r="C193" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A194">
-        <v>51736</v>
-      </c>
-      <c r="B194" s="1">
-        <v>2</v>
-      </c>
-      <c r="C194" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195">
-        <v>21469</v>
       </c>
       <c r="B195" s="1">
         <v>1</v>
       </c>
       <c r="C195" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196">
-        <v>21470</v>
+        <v>51736</v>
       </c>
       <c r="B196" s="1">
         <v>2</v>
       </c>
       <c r="C196" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197">
-        <v>21471</v>
+        <v>21469</v>
       </c>
       <c r="B197" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C197" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198">
-        <v>40949</v>
+        <v>21470</v>
       </c>
       <c r="B198" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C198" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199">
+        <v>21471</v>
+      </c>
+      <c r="B199" s="1">
+        <v>3</v>
+      </c>
+      <c r="C199" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>40949</v>
+      </c>
+      <c r="B200" s="1">
+        <v>4</v>
+      </c>
+      <c r="C200" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201">
         <v>40399</v>
       </c>
-      <c r="B199" s="1">
+      <c r="B201" s="1">
         <v>10</v>
       </c>
-      <c r="C199" s="2" t="s">
+      <c r="C201" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202">
         <v>20957</v>
       </c>
-      <c r="B200" s="1">
+      <c r="B202" s="1">
         <v>1</v>
-      </c>
-      <c r="C200" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201">
-        <v>20956</v>
-      </c>
-      <c r="B201" s="1">
-        <v>2</v>
-      </c>
-      <c r="C201" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A202">
-        <v>20955</v>
-      </c>
-      <c r="B202" s="1">
-        <v>3</v>
       </c>
       <c r="C202" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203">
-        <v>20953</v>
+        <v>20956</v>
       </c>
       <c r="B203" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C203" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204">
-        <v>20952</v>
+        <v>20955</v>
       </c>
       <c r="B204" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C204" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205">
+        <v>20953</v>
+      </c>
+      <c r="B205" s="1">
+        <v>4</v>
+      </c>
+      <c r="C205" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>20952</v>
+      </c>
+      <c r="B206" s="1">
+        <v>5</v>
+      </c>
+      <c r="C206" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>20951</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D207" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208">
         <v>51586</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="B208" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C205" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A206">
-        <v>51587</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C206" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A207">
-        <v>51588</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C207" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A208">
-        <v>51589</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C208" t="s">
         <v>91</v>
@@ -3624,10 +3668,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209">
-        <v>51590</v>
+        <v>51587</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C209" t="s">
         <v>91</v>
@@ -3635,233 +3679,233 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210">
-        <v>40359</v>
+        <v>51588</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C210" t="s">
-        <v>31</v>
-      </c>
-      <c r="D210" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211">
-        <v>19637</v>
+        <v>51589</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C211" t="s">
-        <v>31</v>
-      </c>
-      <c r="D211" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212">
-        <v>19636</v>
+        <v>51590</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C212" t="s">
-        <v>31</v>
-      </c>
-      <c r="D212" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213">
-        <v>19635</v>
+        <v>40358</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C213" t="s">
         <v>31</v>
       </c>
       <c r="D213" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214">
-        <v>19634</v>
+        <v>19632</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C214" t="s">
         <v>31</v>
       </c>
       <c r="D214" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215">
-        <v>40358</v>
+        <v>19631</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C215" t="s">
         <v>31</v>
       </c>
       <c r="D215" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216">
-        <v>19632</v>
+        <v>40359</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C216" t="s">
         <v>31</v>
       </c>
       <c r="D216" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217">
-        <v>19631</v>
+        <v>19637</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C217" t="s">
         <v>31</v>
       </c>
       <c r="D217" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218">
-        <v>19630</v>
+        <v>19636</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C218" t="s">
         <v>31</v>
       </c>
       <c r="D218" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219">
-        <v>19629</v>
+        <v>19635</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C219" t="s">
         <v>31</v>
       </c>
       <c r="D219" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220">
-        <v>48036</v>
+        <v>19634</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="C220" t="s">
-        <v>111</v>
+        <v>31</v>
       </c>
       <c r="D220" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221">
-        <v>405</v>
+        <v>19629</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="C221" t="s">
-        <v>111</v>
+        <v>31</v>
+      </c>
+      <c r="D221" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222">
-        <v>768</v>
+        <v>19630</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="C222" t="s">
-        <v>111</v>
+        <v>31</v>
+      </c>
+      <c r="D222" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223">
-        <v>6664</v>
+        <v>48036</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C223" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D223" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224">
-        <v>6665</v>
+        <v>405</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C224" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225">
-        <v>6666</v>
+        <v>768</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C225" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226">
-        <v>6667</v>
+        <v>6664</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C226" t="s">
         <v>112</v>
       </c>
+      <c r="D226" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227">
-        <v>6668</v>
+        <v>6665</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C227" t="s">
         <v>112</v>
@@ -3869,54 +3913,54 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228">
-        <v>20947</v>
-      </c>
-      <c r="B228" s="1">
-        <v>4</v>
+        <v>6666</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C228" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229">
-        <v>20951</v>
-      </c>
-      <c r="B229" s="1">
-        <v>5</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>38</v>
+        <v>6667</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C229" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230">
-        <v>20942</v>
-      </c>
-      <c r="B230" s="1">
-        <v>1</v>
+        <v>6668</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C230" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231">
-        <v>20945</v>
+        <v>20947</v>
       </c>
       <c r="B231" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C231" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232">
-        <v>20944</v>
+        <v>20942</v>
       </c>
       <c r="B232" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C232" t="s">
         <v>37</v>
@@ -3924,54 +3968,54 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233">
-        <v>23444</v>
+        <v>20945</v>
       </c>
       <c r="B233" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C233" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234">
-        <v>22609</v>
+        <v>20944</v>
       </c>
       <c r="B234" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C234" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235">
-        <v>40954</v>
+        <v>23444</v>
       </c>
       <c r="B235" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C235" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236">
-        <v>40400</v>
+        <v>22609</v>
       </c>
       <c r="B236" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C236" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237">
-        <v>21170</v>
+        <v>40954</v>
       </c>
       <c r="B237" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C237" t="s">
         <v>50</v>
@@ -3979,638 +4023,641 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238">
-        <v>28196</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>13</v>
+        <v>40400</v>
+      </c>
+      <c r="B238" s="1">
+        <v>7</v>
       </c>
       <c r="C238" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239">
-        <v>28197</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>15</v>
+        <v>21170</v>
+      </c>
+      <c r="B239" s="1">
+        <v>8</v>
       </c>
       <c r="C239" t="s">
-        <v>67</v>
-      </c>
-      <c r="D239" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240">
+        <v>28196</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C240" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>28197</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C241" t="s">
+        <v>67</v>
+      </c>
+      <c r="D241" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242">
         <v>28198</v>
       </c>
-      <c r="B240" s="1" t="s">
+      <c r="B242" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C242" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A241">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243">
         <v>28199</v>
       </c>
-      <c r="B241" s="1" t="s">
+      <c r="B243" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C243" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A242">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244">
         <v>28191</v>
       </c>
-      <c r="B242" s="1" t="s">
+      <c r="B244" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C242" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A243">
-        <v>28192</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C243" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A244">
-        <v>28193</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C244" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245">
-        <v>28194</v>
+        <v>28192</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C245" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246">
-        <v>28195</v>
+        <v>28193</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C246" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247">
+        <v>28194</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C247" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>28195</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C248" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249">
         <v>52172</v>
       </c>
-      <c r="B247" s="1">
+      <c r="B249" s="1">
         <v>4</v>
       </c>
-      <c r="C247" s="2" t="s">
+      <c r="C249" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A248">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250">
         <v>47996</v>
       </c>
-      <c r="B248" s="1">
+      <c r="B250" s="1">
         <v>16</v>
-      </c>
-      <c r="C248" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A249">
-        <v>47997</v>
-      </c>
-      <c r="B249" s="1">
-        <v>17</v>
-      </c>
-      <c r="C249" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A250">
-        <v>47998</v>
-      </c>
-      <c r="B250" s="1">
-        <v>18</v>
       </c>
       <c r="C250" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251">
-        <v>47999</v>
+        <v>47997</v>
       </c>
       <c r="B251" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C251" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252">
-        <v>21183</v>
+        <v>47998</v>
       </c>
       <c r="B252" s="1">
+        <v>18</v>
+      </c>
+      <c r="C252" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>47999</v>
+      </c>
+      <c r="B253" s="1">
+        <v>19</v>
+      </c>
+      <c r="C253" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>28671</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C254" t="s">
+        <v>132</v>
+      </c>
+      <c r="D254" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>28670</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C255" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>28673</v>
+      </c>
+      <c r="B256" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C252" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A253">
-        <v>21184</v>
-      </c>
-      <c r="B253" s="1">
-        <v>2</v>
-      </c>
-      <c r="C253" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A254">
-        <v>21185</v>
-      </c>
-      <c r="B254" s="1">
-        <v>3</v>
-      </c>
-      <c r="C254" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A255">
-        <v>21131</v>
-      </c>
-      <c r="B255" s="1">
-        <v>4</v>
-      </c>
-      <c r="C255" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A256">
-        <v>21132</v>
-      </c>
-      <c r="B256" s="1">
-        <v>5</v>
-      </c>
       <c r="C256" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257">
-        <v>27577</v>
-      </c>
-      <c r="B257" s="1">
-        <v>6</v>
+        <v>28674</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C257" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258">
-        <v>51732</v>
-      </c>
-      <c r="B258" s="1">
-        <v>1</v>
+        <v>28675</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C258" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259">
-        <v>51731</v>
+        <v>21183</v>
       </c>
       <c r="B259" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C259" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260">
-        <v>51733</v>
+        <v>21184</v>
       </c>
       <c r="B260" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C260" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261">
-        <v>51734</v>
+        <v>21185</v>
       </c>
       <c r="B261" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C261" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262">
-        <v>47111</v>
+        <v>21131</v>
       </c>
       <c r="B262" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C262" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263">
-        <v>47112</v>
+        <v>21132</v>
       </c>
       <c r="B263" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C263" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264">
-        <v>47113</v>
+        <v>27577</v>
       </c>
       <c r="B264" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C264" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265">
-        <v>21048</v>
+        <v>51732</v>
       </c>
       <c r="B265" s="1">
         <v>1</v>
       </c>
       <c r="C265" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266">
-        <v>47109</v>
+        <v>51731</v>
       </c>
       <c r="B266" s="1">
         <v>2</v>
       </c>
       <c r="C266" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267">
-        <v>47110</v>
+        <v>51733</v>
       </c>
       <c r="B267" s="1">
         <v>3</v>
       </c>
       <c r="C267" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268">
-        <v>47168</v>
+        <v>51734</v>
       </c>
       <c r="B268" s="1">
         <v>4</v>
       </c>
       <c r="C268" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269">
-        <v>35756</v>
-      </c>
-      <c r="B269" s="1" t="s">
-        <v>2</v>
+        <v>47111</v>
+      </c>
+      <c r="B269" s="1">
+        <v>5</v>
       </c>
       <c r="C269" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270">
-        <v>35822</v>
-      </c>
-      <c r="B270" s="1" t="s">
-        <v>3</v>
+        <v>47112</v>
+      </c>
+      <c r="B270" s="1">
+        <v>6</v>
       </c>
       <c r="C270" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271">
-        <v>48368</v>
-      </c>
-      <c r="B271" s="1" t="s">
-        <v>2</v>
+        <v>47113</v>
+      </c>
+      <c r="B271" s="1">
+        <v>7</v>
       </c>
       <c r="C271" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272">
-        <v>22969</v>
-      </c>
-      <c r="B272" s="1" t="s">
+        <v>21048</v>
+      </c>
+      <c r="B272" s="1">
+        <v>1</v>
+      </c>
+      <c r="C272" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>47109</v>
+      </c>
+      <c r="B273" s="1">
+        <v>2</v>
+      </c>
+      <c r="C273" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>47110</v>
+      </c>
+      <c r="B274" s="1">
         <v>3</v>
       </c>
-      <c r="C272" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A273">
-        <v>21611</v>
-      </c>
-      <c r="B273" s="1" t="s">
+      <c r="C274" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>47168</v>
+      </c>
+      <c r="B275" s="1">
         <v>4</v>
       </c>
-      <c r="C273" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A274">
-        <v>19815</v>
-      </c>
-      <c r="B274" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C274" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A275">
-        <v>19814</v>
-      </c>
-      <c r="B275" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="C275" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276">
-        <v>48471</v>
+        <v>35756</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C276" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277">
-        <v>48473</v>
+        <v>35822</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C277" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278">
-        <v>48474</v>
+        <v>48368</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C278" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279">
-        <v>19813</v>
+        <v>22969</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C279" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280">
-        <v>19812</v>
+        <v>21611</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C280" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281">
-        <v>19811</v>
+        <v>19815</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C281" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282">
-        <v>19810</v>
+        <v>19814</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C282" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283">
-        <v>19809</v>
+        <v>48471</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C283" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284">
-        <v>19808</v>
+        <v>48473</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C284" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C284" t="s">
         <v>34</v>
       </c>
-      <c r="D284" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285">
-        <v>19807</v>
+        <v>48474</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C285" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C285" t="s">
         <v>34</v>
       </c>
-      <c r="D285" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286">
-        <v>19806</v>
+        <v>19813</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C286" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C286" t="s">
         <v>34</v>
       </c>
-      <c r="D286" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287">
-        <v>18776</v>
-      </c>
-      <c r="B287" s="1">
-        <v>1</v>
+        <v>19812</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C287" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288">
-        <v>18777</v>
-      </c>
-      <c r="B288" s="1">
-        <v>2</v>
+        <v>19811</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C288" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289">
-        <v>18778</v>
-      </c>
-      <c r="B289" s="1">
-        <v>3</v>
+        <v>19810</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C289" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290">
-        <v>18779</v>
-      </c>
-      <c r="B290" s="1">
-        <v>4</v>
+        <v>19809</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C290" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291">
-        <v>18780</v>
-      </c>
-      <c r="B291" s="1">
-        <v>5</v>
-      </c>
-      <c r="C291" t="s">
-        <v>26</v>
+        <v>19808</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D291" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292">
-        <v>18848</v>
-      </c>
-      <c r="B292" s="1">
+        <v>19807</v>
+      </c>
+      <c r="B292" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C292" t="s">
-        <v>26</v>
+      <c r="C292" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D292" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293">
-        <v>18849</v>
-      </c>
-      <c r="B293" s="1">
-        <v>7</v>
-      </c>
-      <c r="C293" t="s">
-        <v>26</v>
+        <v>19806</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D293" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294">
-        <v>18850</v>
+        <v>18776</v>
       </c>
       <c r="B294" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C294" t="s">
         <v>26</v>
@@ -4618,10 +4665,10 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295">
-        <v>47703</v>
+        <v>18777</v>
       </c>
       <c r="B295" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C295" t="s">
         <v>26</v>
@@ -4629,445 +4676,445 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296">
-        <v>21294</v>
-      </c>
-      <c r="B296" s="1" t="s">
-        <v>2</v>
+        <v>18778</v>
+      </c>
+      <c r="B296" s="1">
+        <v>3</v>
       </c>
       <c r="C296" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297">
-        <v>42981</v>
-      </c>
-      <c r="B297" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C297" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D297" t="s">
-        <v>101</v>
+        <v>18779</v>
+      </c>
+      <c r="B297" s="1">
+        <v>4</v>
+      </c>
+      <c r="C297" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298">
-        <v>42982</v>
-      </c>
-      <c r="B298" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C298" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D298" t="s">
-        <v>101</v>
+        <v>18780</v>
+      </c>
+      <c r="B298" s="1">
+        <v>5</v>
+      </c>
+      <c r="C298" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299">
-        <v>32029</v>
+        <v>18848</v>
       </c>
       <c r="B299" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C299" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300">
-        <v>32028</v>
+        <v>18849</v>
       </c>
       <c r="B300" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C300" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301">
-        <v>32027</v>
+        <v>18850</v>
       </c>
       <c r="B301" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C301" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302">
-        <v>32025</v>
+        <v>47703</v>
       </c>
       <c r="B302" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C302" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303">
-        <v>32026</v>
-      </c>
-      <c r="B303" s="1">
-        <v>5</v>
+        <v>21294</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C303" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304">
+        <v>42981</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D304" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>42982</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D305" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>32029</v>
+      </c>
+      <c r="B306" s="1">
+        <v>1</v>
+      </c>
+      <c r="C306" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>32028</v>
+      </c>
+      <c r="B307" s="1">
+        <v>2</v>
+      </c>
+      <c r="C307" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>32027</v>
+      </c>
+      <c r="B308" s="1">
+        <v>3</v>
+      </c>
+      <c r="C308" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>32025</v>
+      </c>
+      <c r="B309" s="1">
+        <v>4</v>
+      </c>
+      <c r="C309" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>32026</v>
+      </c>
+      <c r="B310" s="1">
+        <v>5</v>
+      </c>
+      <c r="C310" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A311">
         <v>18740</v>
       </c>
-      <c r="B304" s="1">
+      <c r="B311" s="1">
         <v>2</v>
       </c>
-      <c r="C304" t="s">
+      <c r="C311" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A305">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A312">
         <v>18742</v>
       </c>
-      <c r="B305" s="1">
+      <c r="B312" s="1">
         <v>3</v>
       </c>
-      <c r="C305" t="s">
+      <c r="C312" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A306">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A313">
         <v>18741</v>
       </c>
-      <c r="B306" s="1">
+      <c r="B313" s="1">
         <v>5</v>
       </c>
-      <c r="C306" t="s">
+      <c r="C313" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A307">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A314">
         <v>21176</v>
       </c>
-      <c r="B307" s="1">
+      <c r="B314" s="1">
         <v>5</v>
       </c>
-      <c r="C307" s="2" t="s">
+      <c r="C314" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A308">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A315">
         <v>47158</v>
       </c>
-      <c r="B308" s="1">
+      <c r="B315" s="1">
         <v>1</v>
-      </c>
-      <c r="C308" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A309">
-        <v>47159</v>
-      </c>
-      <c r="B309" s="1">
-        <v>2</v>
-      </c>
-      <c r="C309" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A310">
-        <v>47160</v>
-      </c>
-      <c r="B310" s="1">
-        <v>3</v>
-      </c>
-      <c r="C310" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A311">
-        <v>47161</v>
-      </c>
-      <c r="B311" s="1">
-        <v>4</v>
-      </c>
-      <c r="C311" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A312">
-        <v>47162</v>
-      </c>
-      <c r="B312" s="1">
-        <v>5</v>
-      </c>
-      <c r="C312" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A313">
-        <v>47163</v>
-      </c>
-      <c r="B313" s="1">
-        <v>6</v>
-      </c>
-      <c r="C313" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A314">
-        <v>47164</v>
-      </c>
-      <c r="B314" s="1">
-        <v>7</v>
-      </c>
-      <c r="C314" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A315">
-        <v>47165</v>
-      </c>
-      <c r="B315" s="1">
-        <v>8</v>
       </c>
       <c r="C315" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316">
-        <v>47166</v>
+        <v>47159</v>
       </c>
       <c r="B316" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C316" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317">
-        <v>47167</v>
+        <v>47160</v>
       </c>
       <c r="B317" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C317" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318">
-        <v>12964</v>
-      </c>
-      <c r="B318" s="1" t="s">
-        <v>0</v>
+        <v>47161</v>
+      </c>
+      <c r="B318" s="1">
+        <v>4</v>
       </c>
       <c r="C318" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319">
-        <v>19803</v>
-      </c>
-      <c r="B319" s="1" t="s">
-        <v>2</v>
+        <v>47162</v>
+      </c>
+      <c r="B319" s="1">
+        <v>5</v>
       </c>
       <c r="C319" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A320">
-        <v>19804</v>
-      </c>
-      <c r="B320" s="1" t="s">
-        <v>3</v>
+        <v>47163</v>
+      </c>
+      <c r="B320" s="1">
+        <v>6</v>
       </c>
       <c r="C320" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321">
-        <v>19805</v>
-      </c>
-      <c r="B321" s="1" t="s">
-        <v>4</v>
+        <v>47164</v>
+      </c>
+      <c r="B321" s="1">
+        <v>7</v>
       </c>
       <c r="C321" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322">
-        <v>19800</v>
-      </c>
-      <c r="B322" s="1" t="s">
-        <v>1</v>
+        <v>47165</v>
+      </c>
+      <c r="B322" s="1">
+        <v>8</v>
       </c>
       <c r="C322" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323">
-        <v>19231</v>
-      </c>
-      <c r="B323" s="1" t="s">
-        <v>105</v>
+        <v>47166</v>
+      </c>
+      <c r="B323" s="1">
+        <v>9</v>
       </c>
       <c r="C323" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324">
-        <v>18864</v>
-      </c>
-      <c r="B324" s="1" t="s">
-        <v>106</v>
+        <v>47167</v>
+      </c>
+      <c r="B324" s="1">
+        <v>10</v>
       </c>
       <c r="C324" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325">
-        <v>18865</v>
+        <v>12964</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="C325" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326">
-        <v>19228</v>
+        <v>19803</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="C326" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327">
-        <v>19229</v>
+        <v>19804</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="C327" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328">
-        <v>21256</v>
-      </c>
-      <c r="B328" s="1">
-        <v>1</v>
+        <v>19805</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C328" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329">
-        <v>21257</v>
-      </c>
-      <c r="B329" s="1">
-        <v>2</v>
+        <v>19800</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C329" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330">
-        <v>21260</v>
-      </c>
-      <c r="B330" s="1">
-        <v>3</v>
+        <v>19231</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C330" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331">
-        <v>21261</v>
-      </c>
-      <c r="B331" s="1">
-        <v>4</v>
+        <v>18864</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C331" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332">
-        <v>21269</v>
-      </c>
-      <c r="B332" s="1">
-        <v>5</v>
+        <v>18865</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C332" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333">
-        <v>21270</v>
-      </c>
-      <c r="B333" s="1">
-        <v>6</v>
+        <v>19228</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C333" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334">
-        <v>47252</v>
-      </c>
-      <c r="B334" s="1">
-        <v>8</v>
+        <v>19229</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C334" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335">
-        <v>49468</v>
+        <v>21256</v>
       </c>
       <c r="B335" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C335" t="s">
         <v>43</v>
@@ -5075,266 +5122,266 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336">
-        <v>21318</v>
+        <v>21257</v>
       </c>
       <c r="B336" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C336" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337">
-        <v>21005</v>
+        <v>21260</v>
       </c>
       <c r="B337" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C337" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338">
+        <v>21261</v>
+      </c>
+      <c r="B338" s="1">
+        <v>4</v>
+      </c>
+      <c r="C338" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A339">
+        <v>21269</v>
+      </c>
+      <c r="B339" s="1">
+        <v>5</v>
+      </c>
+      <c r="C339" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A340">
+        <v>21270</v>
+      </c>
+      <c r="B340" s="1">
+        <v>6</v>
+      </c>
+      <c r="C340" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A341">
+        <v>47252</v>
+      </c>
+      <c r="B341" s="1">
+        <v>8</v>
+      </c>
+      <c r="C341" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A342">
+        <v>49468</v>
+      </c>
+      <c r="B342" s="1">
+        <v>9</v>
+      </c>
+      <c r="C342" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A343">
+        <v>21318</v>
+      </c>
+      <c r="B343" s="1">
+        <v>10</v>
+      </c>
+      <c r="C343" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A344">
+        <v>21005</v>
+      </c>
+      <c r="B344" s="1">
+        <v>11</v>
+      </c>
+      <c r="C344" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A345">
         <v>46393</v>
       </c>
-      <c r="B338" s="1">
+      <c r="B345" s="1">
         <v>1</v>
-      </c>
-      <c r="C338" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A339">
-        <v>46395</v>
-      </c>
-      <c r="B339" s="1">
-        <v>2</v>
-      </c>
-      <c r="C339" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A340">
-        <v>46396</v>
-      </c>
-      <c r="B340" s="1">
-        <v>3</v>
-      </c>
-      <c r="C340" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A341">
-        <v>46394</v>
-      </c>
-      <c r="B341" s="1">
-        <v>5</v>
-      </c>
-      <c r="C341" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A342">
-        <v>46398</v>
-      </c>
-      <c r="B342" s="1">
-        <v>6</v>
-      </c>
-      <c r="C342" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A343">
-        <v>46399</v>
-      </c>
-      <c r="B343" s="1">
-        <v>7</v>
-      </c>
-      <c r="C343" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A344">
-        <v>46397</v>
-      </c>
-      <c r="B344" s="1">
-        <v>8</v>
-      </c>
-      <c r="C344" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A345">
-        <v>51199</v>
-      </c>
-      <c r="B345" s="1">
-        <v>9</v>
       </c>
       <c r="C345" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346">
-        <v>46401</v>
+        <v>46395</v>
       </c>
       <c r="B346" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C346" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347">
-        <v>46402</v>
+        <v>46396</v>
       </c>
       <c r="B347" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C347" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348">
-        <v>46403</v>
+        <v>46394</v>
       </c>
       <c r="B348" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C348" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349">
-        <v>23175</v>
+        <v>46398</v>
       </c>
       <c r="B349" s="1">
-        <v>51</v>
-      </c>
-      <c r="C349" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D349" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="C349" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350">
-        <v>23183</v>
+        <v>46399</v>
       </c>
       <c r="B350" s="1">
-        <v>74</v>
-      </c>
-      <c r="C350" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="C350" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351">
-        <v>23173</v>
+        <v>46397</v>
       </c>
       <c r="B351" s="1">
-        <v>75</v>
-      </c>
-      <c r="C351" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="C351" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352">
-        <v>20983</v>
+        <v>51199</v>
       </c>
       <c r="B352" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C352" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A353">
-        <v>20984</v>
+        <v>46401</v>
       </c>
       <c r="B353" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C353" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A354">
-        <v>20985</v>
+        <v>46402</v>
       </c>
       <c r="B354" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C354" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A355">
-        <v>20986</v>
+        <v>46403</v>
       </c>
       <c r="B355" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C355" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A356">
-        <v>20987</v>
+        <v>23175</v>
       </c>
       <c r="B356" s="1">
-        <v>5</v>
-      </c>
-      <c r="C356" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D356" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357">
-        <v>20988</v>
+        <v>23183</v>
       </c>
       <c r="B357" s="1">
-        <v>6</v>
-      </c>
-      <c r="C357" t="s">
-        <v>41</v>
+        <v>74</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358">
-        <v>20989</v>
+        <v>23173</v>
       </c>
       <c r="B358" s="1">
-        <v>7</v>
-      </c>
-      <c r="C358" t="s">
-        <v>41</v>
+        <v>75</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A359">
-        <v>20990</v>
+        <v>20983</v>
       </c>
       <c r="B359" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C359" t="s">
         <v>41</v>
@@ -5342,10 +5389,10 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A360">
-        <v>20991</v>
+        <v>20984</v>
       </c>
       <c r="B360" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C360" t="s">
         <v>41</v>
@@ -5353,266 +5400,266 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361">
-        <v>41461</v>
+        <v>20985</v>
       </c>
       <c r="B361" s="1">
-        <v>1</v>
-      </c>
-      <c r="C361" s="2" t="s">
-        <v>102</v>
+        <v>3</v>
+      </c>
+      <c r="C361" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362">
-        <v>41462</v>
+        <v>20986</v>
       </c>
       <c r="B362" s="1">
-        <v>2</v>
-      </c>
-      <c r="C362" s="2" t="s">
-        <v>102</v>
+        <v>4</v>
+      </c>
+      <c r="C362" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363">
-        <v>41463</v>
+        <v>20987</v>
       </c>
       <c r="B363" s="1">
-        <v>3</v>
-      </c>
-      <c r="C363" s="2" t="s">
-        <v>102</v>
+        <v>5</v>
+      </c>
+      <c r="C363" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364">
-        <v>41464</v>
+        <v>20988</v>
       </c>
       <c r="B364" s="1">
-        <v>4</v>
-      </c>
-      <c r="C364" s="2" t="s">
-        <v>102</v>
+        <v>6</v>
+      </c>
+      <c r="C364" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365">
-        <v>41465</v>
+        <v>20989</v>
       </c>
       <c r="B365" s="1">
-        <v>5</v>
-      </c>
-      <c r="C365" s="2" t="s">
-        <v>102</v>
+        <v>7</v>
+      </c>
+      <c r="C365" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A366">
-        <v>41466</v>
+        <v>20990</v>
       </c>
       <c r="B366" s="1">
-        <v>6</v>
-      </c>
-      <c r="C366" s="2" t="s">
-        <v>102</v>
+        <v>8</v>
+      </c>
+      <c r="C366" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A367">
-        <v>21314</v>
+        <v>20991</v>
       </c>
       <c r="B367" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C367" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A368">
+        <v>41461</v>
+      </c>
+      <c r="B368" s="1">
+        <v>1</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A369">
+        <v>41462</v>
+      </c>
+      <c r="B369" s="1">
+        <v>2</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A370">
+        <v>41463</v>
+      </c>
+      <c r="B370" s="1">
+        <v>3</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A371">
+        <v>41464</v>
+      </c>
+      <c r="B371" s="1">
+        <v>4</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A372">
+        <v>41465</v>
+      </c>
+      <c r="B372" s="1">
+        <v>5</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A373">
+        <v>41466</v>
+      </c>
+      <c r="B373" s="1">
+        <v>6</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A374">
+        <v>21314</v>
+      </c>
+      <c r="B374" s="1">
+        <v>1</v>
+      </c>
+      <c r="C374" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A375">
         <v>21315</v>
       </c>
-      <c r="B368" s="1">
+      <c r="B375" s="1">
         <v>2</v>
       </c>
-      <c r="C368" t="s">
+      <c r="C375" t="s">
         <v>59</v>
       </c>
-      <c r="D368" t="s">
+      <c r="D375" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A369">
+    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A376">
         <v>21316</v>
       </c>
-      <c r="B369" s="1">
+      <c r="B376" s="1">
         <v>3</v>
       </c>
-      <c r="C369" t="s">
+      <c r="C376" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A370">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A377">
         <v>20816</v>
-      </c>
-      <c r="B370" s="1">
-        <v>1</v>
-      </c>
-      <c r="C370" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A371">
-        <v>18754</v>
-      </c>
-      <c r="B371" s="1">
-        <v>2</v>
-      </c>
-      <c r="C371" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A372">
-        <v>18755</v>
-      </c>
-      <c r="B372" s="1">
-        <v>3</v>
-      </c>
-      <c r="C372" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A373">
-        <v>18758</v>
-      </c>
-      <c r="B373" s="1">
-        <v>4</v>
-      </c>
-      <c r="C373" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A374">
-        <v>22341</v>
-      </c>
-      <c r="B374" s="1">
-        <v>5</v>
-      </c>
-      <c r="C374" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A375">
-        <v>18759</v>
-      </c>
-      <c r="B375" s="1">
-        <v>6</v>
-      </c>
-      <c r="C375" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A376">
-        <v>18760</v>
-      </c>
-      <c r="B376" s="1">
-        <v>7</v>
-      </c>
-      <c r="C376" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A377">
-        <v>18765</v>
       </c>
       <c r="B377" s="1">
         <v>1</v>
       </c>
       <c r="C377" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A378">
-        <v>18750</v>
+        <v>18754</v>
       </c>
       <c r="B378" s="1">
         <v>2</v>
       </c>
       <c r="C378" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A379">
-        <v>40947</v>
+        <v>18755</v>
       </c>
       <c r="B379" s="1">
         <v>3</v>
       </c>
       <c r="C379" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A380">
-        <v>40946</v>
+        <v>18758</v>
       </c>
       <c r="B380" s="1">
         <v>4</v>
       </c>
       <c r="C380" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A381">
-        <v>18749</v>
+        <v>22341</v>
       </c>
       <c r="B381" s="1">
         <v>5</v>
       </c>
       <c r="C381" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A382">
-        <v>18766</v>
+        <v>18759</v>
       </c>
       <c r="B382" s="1">
         <v>6</v>
       </c>
       <c r="C382" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A383">
-        <v>18761</v>
+        <v>18760</v>
       </c>
       <c r="B383" s="1">
         <v>7</v>
       </c>
       <c r="C383" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A384">
-        <v>18752</v>
+        <v>18765</v>
       </c>
       <c r="B384" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C384" t="s">
         <v>24</v>
@@ -5620,10 +5667,10 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A385">
-        <v>18751</v>
+        <v>18750</v>
       </c>
       <c r="B385" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C385" t="s">
         <v>24</v>
@@ -5631,10 +5678,10 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A386">
-        <v>18763</v>
+        <v>40947</v>
       </c>
       <c r="B386" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C386" t="s">
         <v>24</v>
@@ -5642,10 +5689,10 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A387">
-        <v>18762</v>
+        <v>40946</v>
       </c>
       <c r="B387" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C387" t="s">
         <v>24</v>
@@ -5653,10 +5700,10 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A388">
-        <v>18764</v>
+        <v>18749</v>
       </c>
       <c r="B388" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C388" t="s">
         <v>24</v>
@@ -5664,10 +5711,10 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A389">
-        <v>22342</v>
+        <v>18766</v>
       </c>
       <c r="B389" s="1">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C389" t="s">
         <v>24</v>
@@ -5675,402 +5722,707 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A390">
-        <v>50255</v>
+        <v>18761</v>
       </c>
       <c r="B390" s="1">
-        <v>1</v>
-      </c>
-      <c r="C390" s="2" t="s">
-        <v>97</v>
+        <v>7</v>
+      </c>
+      <c r="C390" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A391">
-        <v>50256</v>
+        <v>18752</v>
       </c>
       <c r="B391" s="1">
-        <v>2</v>
-      </c>
-      <c r="C391" s="2" t="s">
-        <v>97</v>
+        <v>8</v>
+      </c>
+      <c r="C391" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A392">
-        <v>50257</v>
+        <v>18751</v>
       </c>
       <c r="B392" s="1">
-        <v>3</v>
-      </c>
-      <c r="C392" s="2" t="s">
-        <v>97</v>
+        <v>9</v>
+      </c>
+      <c r="C392" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A393">
-        <v>50258</v>
+        <v>18763</v>
       </c>
       <c r="B393" s="1">
-        <v>4</v>
-      </c>
-      <c r="C393" s="2" t="s">
-        <v>97</v>
+        <v>10</v>
+      </c>
+      <c r="C393" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A394">
-        <v>50259</v>
+        <v>18762</v>
       </c>
       <c r="B394" s="1">
-        <v>5</v>
-      </c>
-      <c r="C394" s="2" t="s">
-        <v>97</v>
+        <v>11</v>
+      </c>
+      <c r="C394" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A395">
-        <v>50260</v>
+        <v>18764</v>
       </c>
       <c r="B395" s="1">
-        <v>6</v>
-      </c>
-      <c r="C395" s="2" t="s">
-        <v>97</v>
+        <v>12</v>
+      </c>
+      <c r="C395" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A396">
-        <v>19555</v>
+        <v>22342</v>
       </c>
       <c r="B396" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C396" t="s">
-        <v>29</v>
-      </c>
-      <c r="D396" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A397">
-        <v>47668</v>
-      </c>
-      <c r="B397" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C397" t="s">
-        <v>108</v>
+        <v>50255</v>
+      </c>
+      <c r="B397" s="1">
+        <v>1</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A398">
-        <v>47669</v>
-      </c>
-      <c r="B398" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C398" t="s">
-        <v>108</v>
+        <v>50256</v>
+      </c>
+      <c r="B398" s="1">
+        <v>2</v>
+      </c>
+      <c r="C398" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D398" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A399">
-        <v>47670</v>
-      </c>
-      <c r="B399" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C399" t="s">
-        <v>108</v>
+        <v>50257</v>
+      </c>
+      <c r="B399" s="1">
+        <v>3</v>
+      </c>
+      <c r="C399" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A400">
-        <v>21129</v>
+        <v>50258</v>
       </c>
       <c r="B400" s="1">
+        <v>4</v>
+      </c>
+      <c r="C400" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A401">
+        <v>50259</v>
+      </c>
+      <c r="B401" s="1">
+        <v>5</v>
+      </c>
+      <c r="C401" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A402">
+        <v>27986</v>
+      </c>
+      <c r="B402" s="3">
+        <v>6</v>
+      </c>
+      <c r="C402" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <v>50260</v>
+      </c>
+      <c r="B403" s="3">
+        <v>7</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <v>27985</v>
+      </c>
+      <c r="B404" s="1">
+        <v>8</v>
+      </c>
+      <c r="C404" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <v>27539</v>
+      </c>
+      <c r="B405" s="3">
+        <v>9</v>
+      </c>
+      <c r="C405" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D405" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <v>28543</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C406" t="s">
+        <v>137</v>
+      </c>
+      <c r="D406" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <v>28542</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C407" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <v>28541</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C408" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A409">
+        <v>28540</v>
+      </c>
+      <c r="B409" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C400" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A401">
-        <v>21128</v>
-      </c>
-      <c r="B401" s="1">
+      <c r="C409" t="s">
+        <v>137</v>
+      </c>
+      <c r="D409" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A410">
+        <v>28539</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C410" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A411">
+        <v>28538</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C411" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A412">
+        <v>28537</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C412" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A413">
+        <v>19555</v>
+      </c>
+      <c r="B413" s="1">
         <v>2</v>
       </c>
-      <c r="C401" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A402">
-        <v>40693</v>
-      </c>
-      <c r="B402" s="1">
+      <c r="C413" t="s">
+        <v>29</v>
+      </c>
+      <c r="D413" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A414">
+        <v>47668</v>
+      </c>
+      <c r="B414" s="3">
+        <v>1</v>
+      </c>
+      <c r="C414" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A415">
+        <v>47669</v>
+      </c>
+      <c r="B415" s="3">
+        <v>2</v>
+      </c>
+      <c r="C415" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A416">
+        <v>47670</v>
+      </c>
+      <c r="B416" s="3">
         <v>3</v>
       </c>
-      <c r="C402" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A403">
-        <v>21130</v>
-      </c>
-      <c r="B403" s="1">
-        <v>4</v>
-      </c>
-      <c r="C403" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A404">
-        <v>23278</v>
-      </c>
-      <c r="B404" s="1">
-        <v>5</v>
-      </c>
-      <c r="C404" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A405">
-        <v>23418</v>
-      </c>
-      <c r="B405" s="1">
-        <v>6</v>
-      </c>
-      <c r="C405" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A406">
-        <v>47644</v>
-      </c>
-      <c r="B406" s="1">
-        <v>7</v>
-      </c>
-      <c r="C406" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A407">
-        <v>20965</v>
-      </c>
-      <c r="B407" s="1">
-        <v>1</v>
-      </c>
-      <c r="C407" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A408">
-        <v>20972</v>
-      </c>
-      <c r="B408" s="1">
-        <v>2</v>
-      </c>
-      <c r="C408" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A409">
-        <v>20970</v>
-      </c>
-      <c r="B409" s="1">
-        <v>3</v>
-      </c>
-      <c r="C409" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A410">
-        <v>20968</v>
-      </c>
-      <c r="B410" s="1">
-        <v>4</v>
-      </c>
-      <c r="C410" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A411">
-        <v>20967</v>
-      </c>
-      <c r="B411" s="1">
-        <v>5</v>
-      </c>
-      <c r="C411" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A412">
-        <v>20971</v>
-      </c>
-      <c r="B412" s="1">
-        <v>6</v>
-      </c>
-      <c r="C412" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A413">
-        <v>44766</v>
-      </c>
-      <c r="B413" s="1">
-        <v>7</v>
-      </c>
-      <c r="C413" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A414">
-        <v>46697</v>
-      </c>
-      <c r="B414" s="1">
-        <v>1</v>
-      </c>
-      <c r="C414" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A415">
-        <v>46696</v>
-      </c>
-      <c r="B415" s="1">
-        <v>2</v>
-      </c>
-      <c r="C415" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A416">
-        <v>46698</v>
-      </c>
-      <c r="B416" s="1">
-        <v>3</v>
-      </c>
       <c r="C416" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417">
-        <v>46700</v>
+        <v>21129</v>
       </c>
       <c r="B417" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C417" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418">
-        <v>46701</v>
+        <v>21128</v>
       </c>
       <c r="B418" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C418" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419">
-        <v>50261</v>
+        <v>40693</v>
       </c>
       <c r="B419" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C419" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420">
-        <v>50262</v>
+        <v>21130</v>
       </c>
       <c r="B420" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C420" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421">
-        <v>50263</v>
+        <v>23278</v>
       </c>
       <c r="B421" s="1">
-        <v>3</v>
-      </c>
-      <c r="C421" s="2" t="s">
-        <v>89</v>
+        <v>5</v>
+      </c>
+      <c r="C421" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422">
-        <v>50265</v>
+        <v>23418</v>
       </c>
       <c r="B422" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C422" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423">
-        <v>50266</v>
+        <v>47644</v>
       </c>
       <c r="B423" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C423" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424">
+        <v>47120</v>
+      </c>
+      <c r="B424" s="3">
+        <v>1</v>
+      </c>
+      <c r="C424" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>47121</v>
+      </c>
+      <c r="B425" s="3">
+        <v>2</v>
+      </c>
+      <c r="C425" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>47122</v>
+      </c>
+      <c r="B426" s="3">
+        <v>3</v>
+      </c>
+      <c r="C426" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A427">
+        <v>47123</v>
+      </c>
+      <c r="B427" s="3">
+        <v>4</v>
+      </c>
+      <c r="C427" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <v>47124</v>
+      </c>
+      <c r="B428" s="3">
+        <v>5</v>
+      </c>
+      <c r="C428" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <v>47125</v>
+      </c>
+      <c r="B429" s="3">
+        <v>6</v>
+      </c>
+      <c r="C429" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>47126</v>
+      </c>
+      <c r="B430" s="3">
+        <v>7</v>
+      </c>
+      <c r="C430" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>47700</v>
+      </c>
+      <c r="B431" s="3">
+        <v>8</v>
+      </c>
+      <c r="C431" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>47701</v>
+      </c>
+      <c r="B432" s="3">
+        <v>9</v>
+      </c>
+      <c r="C432" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>20965</v>
+      </c>
+      <c r="B433" s="1">
+        <v>1</v>
+      </c>
+      <c r="C433" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <v>20972</v>
+      </c>
+      <c r="B434" s="1">
+        <v>2</v>
+      </c>
+      <c r="C434" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <v>20970</v>
+      </c>
+      <c r="B435" s="1">
+        <v>3</v>
+      </c>
+      <c r="C435" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A436">
+        <v>20968</v>
+      </c>
+      <c r="B436" s="1">
+        <v>4</v>
+      </c>
+      <c r="C436" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A437">
+        <v>20967</v>
+      </c>
+      <c r="B437" s="1">
+        <v>5</v>
+      </c>
+      <c r="C437" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <v>20971</v>
+      </c>
+      <c r="B438" s="1">
+        <v>6</v>
+      </c>
+      <c r="C438" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <v>44766</v>
+      </c>
+      <c r="B439" s="1">
+        <v>7</v>
+      </c>
+      <c r="C439" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <v>46697</v>
+      </c>
+      <c r="B440" s="1">
+        <v>1</v>
+      </c>
+      <c r="C440" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <v>46696</v>
+      </c>
+      <c r="B441" s="1">
+        <v>2</v>
+      </c>
+      <c r="C441" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A442">
+        <v>46698</v>
+      </c>
+      <c r="B442" s="1">
+        <v>3</v>
+      </c>
+      <c r="C442" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A443">
+        <v>46700</v>
+      </c>
+      <c r="B443" s="1">
+        <v>4</v>
+      </c>
+      <c r="C443" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A444">
+        <v>46701</v>
+      </c>
+      <c r="B444" s="1">
+        <v>5</v>
+      </c>
+      <c r="C444" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A445">
+        <v>50261</v>
+      </c>
+      <c r="B445" s="1">
+        <v>1</v>
+      </c>
+      <c r="C445" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A446">
+        <v>50262</v>
+      </c>
+      <c r="B446" s="1">
+        <v>2</v>
+      </c>
+      <c r="C446" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A447">
+        <v>50263</v>
+      </c>
+      <c r="B447" s="1">
+        <v>3</v>
+      </c>
+      <c r="C447" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D447" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A448">
+        <v>50265</v>
+      </c>
+      <c r="B448" s="1">
+        <v>5</v>
+      </c>
+      <c r="C448" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A449">
+        <v>50266</v>
+      </c>
+      <c r="B449" s="1">
+        <v>6</v>
+      </c>
+      <c r="C449" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A450">
         <v>50267</v>
       </c>
-      <c r="B424" s="1">
+      <c r="B450" s="1">
         <v>7</v>
       </c>
-      <c r="C424" t="s">
+      <c r="C450" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C413" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C413">
-      <sortCondition ref="C1:C413"/>
+  <autoFilter ref="A1:C416" xr:uid="{7250BB86-537C-E141-8619-6288ABCBA058}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C416">
+      <sortCondition ref="C1:C416"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D424">
-    <sortCondition ref="C2:C424"/>
-    <sortCondition ref="B2:B424"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D450">
+    <sortCondition ref="C2:C450"/>
+    <sortCondition ref="B2:B450"/>
   </sortState>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="B207" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>